<commit_message>
Added blood and green condemned trim
</commit_message>
<xml_diff>
--- a/CustomLabelPrinter/src/paperwork/recap.xlsx
+++ b/CustomLabelPrinter/src/paperwork/recap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\pdgwinterm7\git\repository\CustomLabelPrinter\src\paperwork\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdphu\git\customlabelprinter\CustomLabelPrinter\src\paperwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A67FC0-8E5D-414D-9A8F-17728A6851D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7094907F-63B8-41FB-80D0-7BFDC8CA68F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="10740" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8925" yWindow="825" windowWidth="25740" windowHeight="15975" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BREAST" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t>Total Tender Condemned</t>
+  </si>
+  <si>
+    <t>Blood</t>
+  </si>
+  <si>
+    <t>Green</t>
   </si>
 </sst>
 </file>
@@ -618,6 +624,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -630,23 +637,47 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -684,43 +715,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1018,54 +1024,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="35.25" x14ac:dyDescent="0.25">
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="43"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
     </row>
     <row r="2" spans="2:19" ht="27.75" x14ac:dyDescent="0.4">
       <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="44"/>
-      <c r="F2" s="45" t="s">
+      <c r="E2" s="45"/>
+      <c r="F2" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
       <c r="L2" s="7"/>
       <c r="M2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
       <c r="P2" s="7"/>
     </row>
     <row r="3" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
     </row>
     <row r="4" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E4" s="8">
@@ -1098,10 +1104,10 @@
       <c r="N4" s="8">
         <v>26</v>
       </c>
-      <c r="O4" s="46" t="s">
+      <c r="O4" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="46"/>
+      <c r="P4" s="47"/>
       <c r="R4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1902,57 +1908,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="35.25" x14ac:dyDescent="0.25">
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="43"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
     </row>
     <row r="2" spans="2:19" ht="27.75" x14ac:dyDescent="0.4">
       <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="44"/>
-      <c r="F2" s="45" t="s">
+      <c r="E2" s="45"/>
+      <c r="F2" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
       <c r="L2" s="7"/>
       <c r="M2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
       <c r="P2" s="7"/>
       <c r="S2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
     </row>
     <row r="4" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E4" s="8">
@@ -1985,10 +1991,10 @@
       <c r="N4" s="8">
         <v>26</v>
       </c>
-      <c r="O4" s="46" t="s">
+      <c r="O4" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="46"/>
+      <c r="P4" s="47"/>
     </row>
     <row r="5" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="15"/>
@@ -2783,54 +2789,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="35.25" x14ac:dyDescent="0.25">
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="43"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
     </row>
     <row r="2" spans="2:19" ht="27.75" x14ac:dyDescent="0.4">
       <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="44"/>
-      <c r="F2" s="45" t="s">
+      <c r="E2" s="45"/>
+      <c r="F2" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
       <c r="L2" s="7"/>
       <c r="M2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
       <c r="P2" s="7"/>
     </row>
     <row r="3" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
     </row>
     <row r="4" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E4" s="8">
@@ -2863,20 +2869,20 @@
       <c r="N4" s="8">
         <v>26</v>
       </c>
-      <c r="O4" s="46" t="s">
+      <c r="O4" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="46"/>
+      <c r="P4" s="47"/>
       <c r="S4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="15"/>
-      <c r="C5" s="47">
+      <c r="C5" s="52">
         <v>22486</v>
       </c>
-      <c r="D5" s="48"/>
+      <c r="D5" s="53"/>
       <c r="E5" s="16"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
@@ -2887,13 +2893,13 @@
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
       <c r="N5" s="18"/>
-      <c r="O5" s="65"/>
-      <c r="P5" s="66"/>
+      <c r="O5" s="54"/>
+      <c r="P5" s="55"/>
     </row>
     <row r="6" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="15"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="50"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="49"/>
       <c r="E6" s="19"/>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
@@ -2904,13 +2910,13 @@
       <c r="L6" s="20"/>
       <c r="M6" s="20"/>
       <c r="N6" s="21"/>
-      <c r="O6" s="67"/>
-      <c r="P6" s="68"/>
+      <c r="O6" s="56"/>
+      <c r="P6" s="57"/>
     </row>
     <row r="7" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="15"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="50"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="49"/>
       <c r="E7" s="19"/>
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
@@ -2921,13 +2927,13 @@
       <c r="L7" s="20"/>
       <c r="M7" s="20"/>
       <c r="N7" s="21"/>
-      <c r="O7" s="69"/>
-      <c r="P7" s="70"/>
+      <c r="O7" s="58"/>
+      <c r="P7" s="59"/>
     </row>
     <row r="8" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="15"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="50"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="49"/>
       <c r="E8" s="19"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
@@ -2938,13 +2944,13 @@
       <c r="L8" s="20"/>
       <c r="M8" s="20"/>
       <c r="N8" s="21"/>
-      <c r="O8" s="69"/>
-      <c r="P8" s="70"/>
+      <c r="O8" s="58"/>
+      <c r="P8" s="59"/>
     </row>
     <row r="9" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="15"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="50"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="49"/>
       <c r="E9" s="19"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
@@ -2955,13 +2961,13 @@
       <c r="L9" s="20"/>
       <c r="M9" s="20"/>
       <c r="N9" s="21"/>
-      <c r="O9" s="69"/>
-      <c r="P9" s="70"/>
+      <c r="O9" s="58"/>
+      <c r="P9" s="59"/>
     </row>
     <row r="10" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="15"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="50"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="49"/>
       <c r="E10" s="19"/>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
@@ -2972,13 +2978,13 @@
       <c r="L10" s="20"/>
       <c r="M10" s="20"/>
       <c r="N10" s="21"/>
-      <c r="O10" s="69"/>
-      <c r="P10" s="70"/>
+      <c r="O10" s="58"/>
+      <c r="P10" s="59"/>
     </row>
     <row r="11" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="15"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="50"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="49"/>
       <c r="E11" s="19"/>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
@@ -2989,13 +2995,13 @@
       <c r="L11" s="20"/>
       <c r="M11" s="20"/>
       <c r="N11" s="21"/>
-      <c r="O11" s="69"/>
-      <c r="P11" s="70"/>
+      <c r="O11" s="58"/>
+      <c r="P11" s="59"/>
     </row>
     <row r="12" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="15"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="50"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="49"/>
       <c r="E12" s="19"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
@@ -3006,13 +3012,13 @@
       <c r="L12" s="20"/>
       <c r="M12" s="20"/>
       <c r="N12" s="21"/>
-      <c r="O12" s="69"/>
-      <c r="P12" s="70"/>
+      <c r="O12" s="58"/>
+      <c r="P12" s="59"/>
     </row>
     <row r="13" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="15"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="50"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="49"/>
       <c r="E13" s="19"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
@@ -3023,13 +3029,13 @@
       <c r="L13" s="20"/>
       <c r="M13" s="20"/>
       <c r="N13" s="21"/>
-      <c r="O13" s="69"/>
-      <c r="P13" s="70"/>
+      <c r="O13" s="58"/>
+      <c r="P13" s="59"/>
     </row>
     <row r="14" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="15"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="50"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="49"/>
       <c r="E14" s="19"/>
       <c r="F14" s="20"/>
       <c r="G14" s="20"/>
@@ -3040,13 +3046,13 @@
       <c r="L14" s="20"/>
       <c r="M14" s="20"/>
       <c r="N14" s="21"/>
-      <c r="O14" s="69"/>
-      <c r="P14" s="70"/>
+      <c r="O14" s="58"/>
+      <c r="P14" s="59"/>
     </row>
     <row r="15" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="15"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="50"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="49"/>
       <c r="E15" s="19"/>
       <c r="F15" s="20"/>
       <c r="G15" s="20"/>
@@ -3059,13 +3065,13 @@
       <c r="L15" s="20"/>
       <c r="M15" s="20"/>
       <c r="N15" s="21"/>
-      <c r="O15" s="69"/>
-      <c r="P15" s="70"/>
+      <c r="O15" s="58"/>
+      <c r="P15" s="59"/>
     </row>
     <row r="16" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="15"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="50"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="49"/>
       <c r="E16" s="19"/>
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
@@ -3076,13 +3082,13 @@
       <c r="L16" s="20"/>
       <c r="M16" s="20"/>
       <c r="N16" s="21"/>
-      <c r="O16" s="69"/>
-      <c r="P16" s="70"/>
+      <c r="O16" s="58"/>
+      <c r="P16" s="59"/>
     </row>
     <row r="17" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="15"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="50"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="49"/>
       <c r="E17" s="22"/>
       <c r="F17" s="23"/>
       <c r="G17" s="23"/>
@@ -3093,13 +3099,13 @@
       <c r="L17" s="23"/>
       <c r="M17" s="23"/>
       <c r="N17" s="24"/>
-      <c r="O17" s="69"/>
-      <c r="P17" s="70"/>
+      <c r="O17" s="58"/>
+      <c r="P17" s="59"/>
     </row>
     <row r="18" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="15"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="50"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="49"/>
       <c r="E18" s="11"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
@@ -3110,13 +3116,13 @@
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
       <c r="N18" s="12"/>
-      <c r="O18" s="69"/>
-      <c r="P18" s="70"/>
+      <c r="O18" s="58"/>
+      <c r="P18" s="59"/>
     </row>
     <row r="19" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="15"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="50"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="49"/>
       <c r="E19" s="11"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
@@ -3127,13 +3133,13 @@
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
       <c r="N19" s="12"/>
-      <c r="O19" s="69"/>
-      <c r="P19" s="70"/>
+      <c r="O19" s="58"/>
+      <c r="P19" s="59"/>
     </row>
     <row r="20" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="15"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="50"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="49"/>
       <c r="E20" s="11"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
@@ -3144,13 +3150,13 @@
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
       <c r="N20" s="12"/>
-      <c r="O20" s="69"/>
-      <c r="P20" s="70"/>
+      <c r="O20" s="58"/>
+      <c r="P20" s="59"/>
     </row>
     <row r="21" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="15"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="50"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="49"/>
       <c r="E21" s="11"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -3161,13 +3167,13 @@
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
       <c r="N21" s="12"/>
-      <c r="O21" s="69"/>
-      <c r="P21" s="70"/>
+      <c r="O21" s="58"/>
+      <c r="P21" s="59"/>
     </row>
     <row r="22" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="15"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="50"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="49"/>
       <c r="E22" s="11"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -3178,13 +3184,13 @@
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
       <c r="N22" s="12"/>
-      <c r="O22" s="69"/>
-      <c r="P22" s="70"/>
+      <c r="O22" s="58"/>
+      <c r="P22" s="59"/>
     </row>
     <row r="23" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="15"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="50"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="49"/>
       <c r="E23" s="11"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
@@ -3195,13 +3201,13 @@
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
       <c r="N23" s="12"/>
-      <c r="O23" s="69"/>
-      <c r="P23" s="70"/>
+      <c r="O23" s="58"/>
+      <c r="P23" s="59"/>
     </row>
     <row r="24" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="15"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="50"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="49"/>
       <c r="E24" s="11"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -3212,13 +3218,13 @@
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
       <c r="N24" s="12"/>
-      <c r="O24" s="69"/>
-      <c r="P24" s="70"/>
+      <c r="O24" s="58"/>
+      <c r="P24" s="59"/>
     </row>
     <row r="25" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="15"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="50"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="49"/>
       <c r="E25" s="11"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
@@ -3229,13 +3235,13 @@
       <c r="L25" s="9"/>
       <c r="M25" s="9"/>
       <c r="N25" s="12"/>
-      <c r="O25" s="69"/>
-      <c r="P25" s="70"/>
+      <c r="O25" s="58"/>
+      <c r="P25" s="59"/>
     </row>
     <row r="26" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="15"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="50"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="49"/>
       <c r="E26" s="11"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
@@ -3246,13 +3252,13 @@
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
       <c r="N26" s="12"/>
-      <c r="O26" s="69"/>
-      <c r="P26" s="70"/>
+      <c r="O26" s="58"/>
+      <c r="P26" s="59"/>
     </row>
     <row r="27" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="15"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="52"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="51"/>
       <c r="E27" s="4"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -3263,13 +3269,13 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="13"/>
-      <c r="O27" s="71"/>
-      <c r="P27" s="72"/>
+      <c r="O27" s="60"/>
+      <c r="P27" s="61"/>
     </row>
     <row r="28" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="15"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="48"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="53"/>
       <c r="E28" s="6"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -3280,13 +3286,13 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="10"/>
-      <c r="O28" s="53"/>
-      <c r="P28" s="54"/>
+      <c r="O28" s="62"/>
+      <c r="P28" s="63"/>
     </row>
     <row r="29" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="15"/>
-      <c r="C29" s="49"/>
-      <c r="D29" s="50"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="49"/>
       <c r="E29" s="11"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
@@ -3297,13 +3303,13 @@
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
       <c r="N29" s="12"/>
-      <c r="O29" s="55"/>
-      <c r="P29" s="56"/>
+      <c r="O29" s="64"/>
+      <c r="P29" s="65"/>
     </row>
     <row r="30" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="15"/>
-      <c r="C30" s="49"/>
-      <c r="D30" s="50"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="49"/>
       <c r="E30" s="11"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
@@ -3314,13 +3320,13 @@
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
       <c r="N30" s="12"/>
-      <c r="O30" s="55"/>
-      <c r="P30" s="56"/>
+      <c r="O30" s="64"/>
+      <c r="P30" s="65"/>
     </row>
     <row r="31" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="15"/>
-      <c r="C31" s="49"/>
-      <c r="D31" s="50"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="49"/>
       <c r="E31" s="11"/>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
@@ -3331,13 +3337,13 @@
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
       <c r="N31" s="12"/>
-      <c r="O31" s="55"/>
-      <c r="P31" s="56"/>
+      <c r="O31" s="64"/>
+      <c r="P31" s="65"/>
     </row>
     <row r="32" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="15"/>
-      <c r="C32" s="49"/>
-      <c r="D32" s="50"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="49"/>
       <c r="E32" s="11"/>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
@@ -3348,13 +3354,13 @@
       <c r="L32" s="9"/>
       <c r="M32" s="9"/>
       <c r="N32" s="12"/>
-      <c r="O32" s="55"/>
-      <c r="P32" s="56"/>
+      <c r="O32" s="64"/>
+      <c r="P32" s="65"/>
     </row>
     <row r="33" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="15"/>
-      <c r="C33" s="49"/>
-      <c r="D33" s="50"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="49"/>
       <c r="E33" s="11"/>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
@@ -3365,13 +3371,13 @@
       <c r="L33" s="9"/>
       <c r="M33" s="9"/>
       <c r="N33" s="12"/>
-      <c r="O33" s="55"/>
-      <c r="P33" s="56"/>
+      <c r="O33" s="64"/>
+      <c r="P33" s="65"/>
     </row>
     <row r="34" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="15"/>
-      <c r="C34" s="49"/>
-      <c r="D34" s="50"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="49"/>
       <c r="E34" s="11"/>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
@@ -3382,13 +3388,13 @@
       <c r="L34" s="9"/>
       <c r="M34" s="9"/>
       <c r="N34" s="12"/>
-      <c r="O34" s="55"/>
-      <c r="P34" s="56"/>
+      <c r="O34" s="64"/>
+      <c r="P34" s="65"/>
     </row>
     <row r="35" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="15"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="50"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="49"/>
       <c r="E35" s="11"/>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
@@ -3399,13 +3405,13 @@
       <c r="L35" s="9"/>
       <c r="M35" s="9"/>
       <c r="N35" s="12"/>
-      <c r="O35" s="55"/>
-      <c r="P35" s="56"/>
+      <c r="O35" s="64"/>
+      <c r="P35" s="65"/>
     </row>
     <row r="36" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="15"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="50"/>
+      <c r="C36" s="48"/>
+      <c r="D36" s="49"/>
       <c r="E36" s="11"/>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
@@ -3416,13 +3422,13 @@
       <c r="L36" s="9"/>
       <c r="M36" s="9"/>
       <c r="N36" s="12"/>
-      <c r="O36" s="55"/>
-      <c r="P36" s="56"/>
+      <c r="O36" s="64"/>
+      <c r="P36" s="65"/>
     </row>
     <row r="37" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="15"/>
-      <c r="C37" s="49"/>
-      <c r="D37" s="50"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="49"/>
       <c r="E37" s="11"/>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
@@ -3433,13 +3439,13 @@
       <c r="L37" s="9"/>
       <c r="M37" s="9"/>
       <c r="N37" s="12"/>
-      <c r="O37" s="55"/>
-      <c r="P37" s="56"/>
+      <c r="O37" s="64"/>
+      <c r="P37" s="65"/>
     </row>
     <row r="38" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" s="15"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="52"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="51"/>
       <c r="E38" s="25"/>
       <c r="F38" s="26"/>
       <c r="G38" s="26"/>
@@ -3450,14 +3456,14 @@
       <c r="L38" s="26"/>
       <c r="M38" s="26"/>
       <c r="N38" s="27"/>
-      <c r="O38" s="57"/>
-      <c r="P38" s="58"/>
+      <c r="O38" s="66"/>
+      <c r="P38" s="67"/>
     </row>
     <row r="39" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39"/>
       <c r="B39"/>
-      <c r="C39" s="59"/>
-      <c r="D39" s="60"/>
+      <c r="C39" s="68"/>
+      <c r="D39" s="69"/>
       <c r="E39" s="29"/>
       <c r="F39" s="28"/>
       <c r="G39" s="28"/>
@@ -3468,8 +3474,8 @@
       <c r="L39" s="28"/>
       <c r="M39" s="28"/>
       <c r="N39" s="30"/>
-      <c r="O39" s="59"/>
-      <c r="P39" s="60"/>
+      <c r="O39" s="68"/>
+      <c r="P39" s="69"/>
       <c r="Q39"/>
       <c r="R39"/>
       <c r="S39"/>
@@ -3477,8 +3483,8 @@
     <row r="40" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40"/>
       <c r="B40"/>
-      <c r="C40" s="61"/>
-      <c r="D40" s="62"/>
+      <c r="C40" s="70"/>
+      <c r="D40" s="71"/>
       <c r="E40" s="29"/>
       <c r="F40" s="28"/>
       <c r="G40" s="28"/>
@@ -3489,8 +3495,8 @@
       <c r="L40" s="28"/>
       <c r="M40" s="28"/>
       <c r="N40" s="30"/>
-      <c r="O40" s="61"/>
-      <c r="P40" s="62"/>
+      <c r="O40" s="70"/>
+      <c r="P40" s="71"/>
       <c r="Q40"/>
       <c r="R40"/>
       <c r="S40"/>
@@ -3498,8 +3504,8 @@
     <row r="41" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41"/>
       <c r="B41"/>
-      <c r="C41" s="61"/>
-      <c r="D41" s="62"/>
+      <c r="C41" s="70"/>
+      <c r="D41" s="71"/>
       <c r="E41" s="29"/>
       <c r="F41" s="28"/>
       <c r="G41" s="28"/>
@@ -3510,8 +3516,8 @@
       <c r="L41" s="28"/>
       <c r="M41" s="28"/>
       <c r="N41" s="30"/>
-      <c r="O41" s="61"/>
-      <c r="P41" s="62"/>
+      <c r="O41" s="70"/>
+      <c r="P41" s="71"/>
       <c r="Q41"/>
       <c r="R41"/>
       <c r="S41"/>
@@ -3519,8 +3525,8 @@
     <row r="42" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42"/>
       <c r="B42"/>
-      <c r="C42" s="61"/>
-      <c r="D42" s="62"/>
+      <c r="C42" s="70"/>
+      <c r="D42" s="71"/>
       <c r="E42" s="29"/>
       <c r="F42" s="28"/>
       <c r="G42" s="28"/>
@@ -3531,8 +3537,8 @@
       <c r="L42" s="28"/>
       <c r="M42" s="28"/>
       <c r="N42" s="30"/>
-      <c r="O42" s="61"/>
-      <c r="P42" s="62"/>
+      <c r="O42" s="70"/>
+      <c r="P42" s="71"/>
       <c r="Q42"/>
       <c r="R42"/>
       <c r="S42"/>
@@ -3540,8 +3546,8 @@
     <row r="43" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43"/>
       <c r="B43"/>
-      <c r="C43" s="63"/>
-      <c r="D43" s="64"/>
+      <c r="C43" s="72"/>
+      <c r="D43" s="73"/>
       <c r="E43" s="29"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
@@ -3552,8 +3558,8 @@
       <c r="L43" s="28"/>
       <c r="M43" s="28"/>
       <c r="N43" s="30"/>
-      <c r="O43" s="63"/>
-      <c r="P43" s="64"/>
+      <c r="O43" s="72"/>
+      <c r="P43" s="73"/>
       <c r="Q43"/>
       <c r="R43"/>
       <c r="S43"/>
@@ -3686,6 +3692,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C28:D29"/>
+    <mergeCell ref="C30:D38"/>
+    <mergeCell ref="O28:P38"/>
+    <mergeCell ref="C39:D43"/>
+    <mergeCell ref="O39:P43"/>
     <mergeCell ref="C1:P1"/>
     <mergeCell ref="F2:K3"/>
     <mergeCell ref="N2:O2"/>
@@ -3695,11 +3706,6 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="O5:P6"/>
     <mergeCell ref="O7:P27"/>
-    <mergeCell ref="C28:D29"/>
-    <mergeCell ref="C30:D38"/>
-    <mergeCell ref="O28:P38"/>
-    <mergeCell ref="C39:D43"/>
-    <mergeCell ref="O39:P43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="35" orientation="portrait" r:id="rId1"/>
@@ -3746,84 +3752,84 @@
       <c r="C10" s="36"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="73" t="s">
+      <c r="A13" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="73"/>
-      <c r="C13" s="73" t="s">
+      <c r="B13" s="75"/>
+      <c r="C13" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73" t="s">
+      <c r="D13" s="75"/>
+      <c r="E13" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="73" t="s">
+      <c r="F13" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="73"/>
-      <c r="H13" s="73" t="s">
+      <c r="G13" s="75"/>
+      <c r="H13" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="I13" s="73"/>
+      <c r="I13" s="75"/>
     </row>
     <row r="14" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="73"/>
-      <c r="B14" s="73"/>
-      <c r="C14" s="73"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="73"/>
-      <c r="I14" s="73"/>
+      <c r="A14" s="75"/>
+      <c r="B14" s="75"/>
+      <c r="C14" s="75"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="75"/>
+      <c r="F14" s="75"/>
+      <c r="G14" s="75"/>
+      <c r="H14" s="75"/>
+      <c r="I14" s="75"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="73" t="s">
+      <c r="A15" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="73"/>
-      <c r="C15" s="73"/>
-      <c r="D15" s="73"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="73"/>
-      <c r="G15" s="73"/>
-      <c r="H15" s="73"/>
-      <c r="I15" s="73"/>
+      <c r="B15" s="75"/>
+      <c r="C15" s="75"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="75"/>
+      <c r="I15" s="75"/>
     </row>
     <row r="16" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="73"/>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="73"/>
-      <c r="H16" s="73"/>
-      <c r="I16" s="73"/>
+      <c r="A16" s="75"/>
+      <c r="B16" s="75"/>
+      <c r="C16" s="75"/>
+      <c r="D16" s="75"/>
+      <c r="E16" s="75"/>
+      <c r="F16" s="75"/>
+      <c r="G16" s="75"/>
+      <c r="H16" s="75"/>
+      <c r="I16" s="75"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="73" t="s">
+      <c r="A17" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="73"/>
-      <c r="C17" s="73"/>
-      <c r="D17" s="73"/>
-      <c r="E17" s="73"/>
-      <c r="F17" s="73"/>
-      <c r="G17" s="73"/>
-      <c r="H17" s="73"/>
-      <c r="I17" s="73"/>
+      <c r="B17" s="75"/>
+      <c r="C17" s="75"/>
+      <c r="D17" s="75"/>
+      <c r="E17" s="75"/>
+      <c r="F17" s="75"/>
+      <c r="G17" s="75"/>
+      <c r="H17" s="75"/>
+      <c r="I17" s="75"/>
     </row>
     <row r="18" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="73"/>
-      <c r="B18" s="73"/>
-      <c r="C18" s="73"/>
-      <c r="D18" s="73"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="73"/>
-      <c r="H18" s="73"/>
-      <c r="I18" s="73"/>
+      <c r="A18" s="75"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="75"/>
+      <c r="D18" s="75"/>
+      <c r="E18" s="75"/>
+      <c r="F18" s="75"/>
+      <c r="G18" s="75"/>
+      <c r="H18" s="75"/>
+      <c r="I18" s="75"/>
     </row>
     <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="37"/>
@@ -3831,12 +3837,12 @@
       <c r="C19" s="37"/>
       <c r="D19" s="37"/>
       <c r="E19" s="37"/>
-      <c r="F19" s="73" t="s">
+      <c r="F19" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="73"/>
-      <c r="H19" s="73"/>
-      <c r="I19" s="73"/>
+      <c r="G19" s="75"/>
+      <c r="H19" s="75"/>
+      <c r="I19" s="75"/>
     </row>
     <row r="20" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="37"/>
@@ -3844,106 +3850,106 @@
       <c r="C20" s="37"/>
       <c r="D20" s="37"/>
       <c r="E20" s="37"/>
-      <c r="F20" s="73"/>
-      <c r="G20" s="73"/>
-      <c r="H20" s="73"/>
-      <c r="I20" s="73"/>
+      <c r="F20" s="75"/>
+      <c r="G20" s="75"/>
+      <c r="H20" s="75"/>
+      <c r="I20" s="75"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="73" t="s">
+      <c r="A21" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="73"/>
-      <c r="C21" s="73"/>
-      <c r="D21" s="73"/>
-      <c r="E21" s="73"/>
-      <c r="F21" s="73"/>
-      <c r="G21" s="73"/>
-      <c r="H21" s="73"/>
-      <c r="I21" s="73"/>
+      <c r="B21" s="75"/>
+      <c r="C21" s="75"/>
+      <c r="D21" s="75"/>
+      <c r="E21" s="75"/>
+      <c r="F21" s="75"/>
+      <c r="G21" s="75"/>
+      <c r="H21" s="75"/>
+      <c r="I21" s="75"/>
     </row>
     <row r="22" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="73"/>
-      <c r="B22" s="73"/>
-      <c r="C22" s="73"/>
-      <c r="D22" s="73"/>
-      <c r="E22" s="73"/>
-      <c r="F22" s="73"/>
-      <c r="G22" s="73"/>
-      <c r="H22" s="73"/>
-      <c r="I22" s="73"/>
+      <c r="A22" s="75"/>
+      <c r="B22" s="75"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="75"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="75"/>
+      <c r="I22" s="75"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="73" t="s">
+      <c r="A23" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="73"/>
-      <c r="C23" s="73"/>
-      <c r="D23" s="73"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="73"/>
-      <c r="H23" s="73"/>
-      <c r="I23" s="73"/>
+      <c r="B23" s="75"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="75"/>
+      <c r="I23" s="75"/>
     </row>
     <row r="24" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="73"/>
-      <c r="B24" s="73"/>
-      <c r="C24" s="73"/>
-      <c r="D24" s="73"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="73"/>
-      <c r="G24" s="73"/>
-      <c r="H24" s="73"/>
-      <c r="I24" s="73"/>
+      <c r="A24" s="75"/>
+      <c r="B24" s="75"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="75"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="75"/>
+      <c r="I24" s="75"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="73" t="s">
+      <c r="A25" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="73"/>
-      <c r="C25" s="73"/>
-      <c r="D25" s="73"/>
-      <c r="E25" s="73"/>
-      <c r="F25" s="73"/>
-      <c r="G25" s="73"/>
-      <c r="H25" s="73"/>
-      <c r="I25" s="73"/>
+      <c r="B25" s="75"/>
+      <c r="C25" s="75"/>
+      <c r="D25" s="75"/>
+      <c r="E25" s="75"/>
+      <c r="F25" s="75"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="75"/>
+      <c r="I25" s="75"/>
     </row>
     <row r="26" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="73"/>
-      <c r="B26" s="73"/>
-      <c r="C26" s="73"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="73"/>
-      <c r="F26" s="73"/>
-      <c r="G26" s="73"/>
-      <c r="H26" s="73"/>
-      <c r="I26" s="73"/>
+      <c r="A26" s="75"/>
+      <c r="B26" s="75"/>
+      <c r="C26" s="75"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="75"/>
+      <c r="F26" s="75"/>
+      <c r="G26" s="75"/>
+      <c r="H26" s="75"/>
+      <c r="I26" s="75"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="73" t="s">
+      <c r="A27" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="73"/>
-      <c r="C27" s="73"/>
-      <c r="D27" s="73"/>
-      <c r="E27" s="73"/>
-      <c r="F27" s="73"/>
-      <c r="G27" s="73"/>
-      <c r="H27" s="73"/>
-      <c r="I27" s="73"/>
+      <c r="B27" s="75"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="75"/>
+      <c r="F27" s="75"/>
+      <c r="G27" s="75"/>
+      <c r="H27" s="75"/>
+      <c r="I27" s="75"/>
     </row>
     <row r="28" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="73"/>
-      <c r="B28" s="73"/>
-      <c r="C28" s="73"/>
-      <c r="D28" s="73"/>
-      <c r="E28" s="73"/>
-      <c r="F28" s="73"/>
-      <c r="G28" s="73"/>
-      <c r="H28" s="73"/>
-      <c r="I28" s="73"/>
+      <c r="A28" s="75"/>
+      <c r="B28" s="75"/>
+      <c r="C28" s="75"/>
+      <c r="D28" s="75"/>
+      <c r="E28" s="75"/>
+      <c r="F28" s="75"/>
+      <c r="G28" s="75"/>
+      <c r="H28" s="75"/>
+      <c r="I28" s="75"/>
     </row>
     <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="38" t="s">
@@ -3954,34 +3960,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="A25:B26"/>
-    <mergeCell ref="C25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:G26"/>
-    <mergeCell ref="H25:I26"/>
-    <mergeCell ref="A27:B28"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:G28"/>
-    <mergeCell ref="H27:I28"/>
-    <mergeCell ref="F19:G20"/>
-    <mergeCell ref="H19:I20"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="C17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:G18"/>
-    <mergeCell ref="H17:I18"/>
-    <mergeCell ref="A21:B22"/>
-    <mergeCell ref="C21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:G22"/>
-    <mergeCell ref="H21:I22"/>
-    <mergeCell ref="A23:B24"/>
-    <mergeCell ref="C23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:G24"/>
-    <mergeCell ref="H23:I24"/>
     <mergeCell ref="F13:G14"/>
     <mergeCell ref="H13:I14"/>
     <mergeCell ref="A15:B16"/>
@@ -3992,6 +3970,34 @@
     <mergeCell ref="A13:B14"/>
     <mergeCell ref="C13:D14"/>
     <mergeCell ref="E13:E14"/>
+    <mergeCell ref="A23:B24"/>
+    <mergeCell ref="C23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:G24"/>
+    <mergeCell ref="H23:I24"/>
+    <mergeCell ref="A21:B22"/>
+    <mergeCell ref="C21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:G22"/>
+    <mergeCell ref="H21:I22"/>
+    <mergeCell ref="F19:G20"/>
+    <mergeCell ref="H19:I20"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="C17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:G18"/>
+    <mergeCell ref="H17:I18"/>
+    <mergeCell ref="H25:I26"/>
+    <mergeCell ref="A27:B28"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:G28"/>
+    <mergeCell ref="H27:I28"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="A25:B26"/>
+    <mergeCell ref="C25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:G26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4002,8 +4008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A016E41C-E536-466F-8BCC-D27E2EA7F174}">
   <dimension ref="A3:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4017,22 +4023,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="75"/>
-      <c r="G3" s="75" t="s">
+      <c r="B3" s="76"/>
+      <c r="G3" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
     </row>
     <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G5" s="76" t="s">
+      <c r="G5" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="76"/>
-      <c r="I5" s="76"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
     </row>
     <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="40" t="s">
@@ -4040,37 +4046,37 @@
       </c>
       <c r="B6" s="42"/>
       <c r="C6" s="39"/>
-      <c r="G6" s="76"/>
-      <c r="H6" s="76"/>
-      <c r="I6" s="76"/>
+      <c r="G6" s="77"/>
+      <c r="H6" s="77"/>
+      <c r="I6" s="77"/>
     </row>
     <row r="7" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="42"/>
       <c r="C7" s="39"/>
-      <c r="G7" s="76"/>
-      <c r="H7" s="76"/>
-      <c r="I7" s="76"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="77"/>
     </row>
     <row r="8" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="42"/>
       <c r="C8" s="39"/>
-      <c r="G8" s="76"/>
-      <c r="H8" s="76"/>
-      <c r="I8" s="76"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="77"/>
+      <c r="I8" s="77"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B9" s="42"/>
       <c r="C9" s="39"/>
-      <c r="G9" s="76"/>
-      <c r="H9" s="76"/>
-      <c r="I9" s="76"/>
+      <c r="G9" s="77"/>
+      <c r="H9" s="77"/>
+      <c r="I9" s="77"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B10" s="42"/>
       <c r="C10" s="39"/>
-      <c r="G10" s="76"/>
-      <c r="H10" s="76"/>
-      <c r="I10" s="76"/>
+      <c r="G10" s="77"/>
+      <c r="H10" s="77"/>
+      <c r="I10" s="77"/>
     </row>
     <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
@@ -4078,9 +4084,9 @@
       </c>
       <c r="B11" s="42"/>
       <c r="C11" s="39"/>
-      <c r="G11" s="76"/>
-      <c r="H11" s="76"/>
-      <c r="I11" s="76"/>
+      <c r="G11" s="77"/>
+      <c r="H11" s="77"/>
+      <c r="I11" s="77"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B12" s="42"/>
@@ -4104,6 +4110,9 @@
       </c>
       <c r="B16" s="42"/>
       <c r="C16" s="39"/>
+      <c r="G16" s="43" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B17" s="42"/>
@@ -4128,12 +4137,14 @@
       <c r="B21" s="42"/>
       <c r="C21" s="39"/>
     </row>
-    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="B22" s="42"/>
       <c r="C22" s="39"/>
-      <c r="G22" s="77" t="s">
-        <v>35</v>
-      </c>
+      <c r="G22" s="76" t="s">
+        <v>31</v>
+      </c>
+      <c r="H22" s="76"/>
+      <c r="I22" s="76"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B23" s="42"/>
@@ -4142,6 +4153,12 @@
     <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B24" s="42"/>
       <c r="C24" s="39"/>
+      <c r="G24" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="I24" s="31" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B25" s="42"/>
@@ -4158,14 +4175,9 @@
       <c r="B27" s="42"/>
       <c r="C27" s="39"/>
     </row>
-    <row r="28" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B28" s="42"/>
       <c r="C28" s="39"/>
-      <c r="G28" s="75" t="s">
-        <v>31</v>
-      </c>
-      <c r="H28" s="75"/>
-      <c r="I28" s="75"/>
     </row>
     <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B29" s="42"/>
@@ -4288,7 +4300,7 @@
   <mergeCells count="4">
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G22:I22"/>
     <mergeCell ref="G5:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adjusted back to 1 condemned trim
</commit_message>
<xml_diff>
--- a/CustomLabelPrinter/src/paperwork/recap.xlsx
+++ b/CustomLabelPrinter/src/paperwork/recap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdphu\git\customlabelprinter\CustomLabelPrinter\src\paperwork\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\pdgwinterm7\git\repository\CustomLabelPrinter\src\paperwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7094907F-63B8-41FB-80D0-7BFDC8CA68F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A67FC0-8E5D-414D-9A8F-17728A6851D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8925" yWindow="825" windowWidth="25740" windowHeight="15975" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="10740" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BREAST" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -137,12 +137,6 @@
   </si>
   <si>
     <t>Total Tender Condemned</t>
-  </si>
-  <si>
-    <t>Blood</t>
-  </si>
-  <si>
-    <t>Green</t>
   </si>
 </sst>
 </file>
@@ -624,7 +618,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -637,6 +630,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -649,11 +648,41 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -679,54 +708,19 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1024,54 +1018,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="35.25" x14ac:dyDescent="0.25">
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
     </row>
     <row r="2" spans="2:19" ht="27.75" x14ac:dyDescent="0.4">
       <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="45"/>
-      <c r="F2" s="46" t="s">
+      <c r="E2" s="44"/>
+      <c r="F2" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
       <c r="L2" s="7"/>
       <c r="M2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
       <c r="P2" s="7"/>
     </row>
     <row r="3" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
     </row>
     <row r="4" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E4" s="8">
@@ -1104,10 +1098,10 @@
       <c r="N4" s="8">
         <v>26</v>
       </c>
-      <c r="O4" s="47" t="s">
+      <c r="O4" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="47"/>
+      <c r="P4" s="46"/>
       <c r="R4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1908,57 +1902,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="35.25" x14ac:dyDescent="0.25">
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
     </row>
     <row r="2" spans="2:19" ht="27.75" x14ac:dyDescent="0.4">
       <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="45"/>
-      <c r="F2" s="46" t="s">
+      <c r="E2" s="44"/>
+      <c r="F2" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
       <c r="L2" s="7"/>
       <c r="M2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
       <c r="P2" s="7"/>
       <c r="S2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
     </row>
     <row r="4" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E4" s="8">
@@ -1991,10 +1985,10 @@
       <c r="N4" s="8">
         <v>26</v>
       </c>
-      <c r="O4" s="47" t="s">
+      <c r="O4" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="47"/>
+      <c r="P4" s="46"/>
     </row>
     <row r="5" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="15"/>
@@ -2789,54 +2783,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="35.25" x14ac:dyDescent="0.25">
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
     </row>
     <row r="2" spans="2:19" ht="27.75" x14ac:dyDescent="0.4">
       <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="45"/>
-      <c r="F2" s="46" t="s">
+      <c r="E2" s="44"/>
+      <c r="F2" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
       <c r="L2" s="7"/>
       <c r="M2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
       <c r="P2" s="7"/>
     </row>
     <row r="3" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
     </row>
     <row r="4" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E4" s="8">
@@ -2869,20 +2863,20 @@
       <c r="N4" s="8">
         <v>26</v>
       </c>
-      <c r="O4" s="47" t="s">
+      <c r="O4" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="47"/>
+      <c r="P4" s="46"/>
       <c r="S4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="15"/>
-      <c r="C5" s="52">
+      <c r="C5" s="47">
         <v>22486</v>
       </c>
-      <c r="D5" s="53"/>
+      <c r="D5" s="48"/>
       <c r="E5" s="16"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
@@ -2893,13 +2887,13 @@
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
       <c r="N5" s="18"/>
-      <c r="O5" s="54"/>
-      <c r="P5" s="55"/>
+      <c r="O5" s="65"/>
+      <c r="P5" s="66"/>
     </row>
     <row r="6" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="15"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="50"/>
       <c r="E6" s="19"/>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
@@ -2910,13 +2904,13 @@
       <c r="L6" s="20"/>
       <c r="M6" s="20"/>
       <c r="N6" s="21"/>
-      <c r="O6" s="56"/>
-      <c r="P6" s="57"/>
+      <c r="O6" s="67"/>
+      <c r="P6" s="68"/>
     </row>
     <row r="7" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="15"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="49"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="50"/>
       <c r="E7" s="19"/>
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
@@ -2927,13 +2921,13 @@
       <c r="L7" s="20"/>
       <c r="M7" s="20"/>
       <c r="N7" s="21"/>
-      <c r="O7" s="58"/>
-      <c r="P7" s="59"/>
+      <c r="O7" s="69"/>
+      <c r="P7" s="70"/>
     </row>
     <row r="8" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="15"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="50"/>
       <c r="E8" s="19"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
@@ -2944,13 +2938,13 @@
       <c r="L8" s="20"/>
       <c r="M8" s="20"/>
       <c r="N8" s="21"/>
-      <c r="O8" s="58"/>
-      <c r="P8" s="59"/>
+      <c r="O8" s="69"/>
+      <c r="P8" s="70"/>
     </row>
     <row r="9" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="15"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="50"/>
       <c r="E9" s="19"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
@@ -2961,13 +2955,13 @@
       <c r="L9" s="20"/>
       <c r="M9" s="20"/>
       <c r="N9" s="21"/>
-      <c r="O9" s="58"/>
-      <c r="P9" s="59"/>
+      <c r="O9" s="69"/>
+      <c r="P9" s="70"/>
     </row>
     <row r="10" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="15"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="50"/>
       <c r="E10" s="19"/>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
@@ -2978,13 +2972,13 @@
       <c r="L10" s="20"/>
       <c r="M10" s="20"/>
       <c r="N10" s="21"/>
-      <c r="O10" s="58"/>
-      <c r="P10" s="59"/>
+      <c r="O10" s="69"/>
+      <c r="P10" s="70"/>
     </row>
     <row r="11" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="15"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="49"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="50"/>
       <c r="E11" s="19"/>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
@@ -2995,13 +2989,13 @@
       <c r="L11" s="20"/>
       <c r="M11" s="20"/>
       <c r="N11" s="21"/>
-      <c r="O11" s="58"/>
-      <c r="P11" s="59"/>
+      <c r="O11" s="69"/>
+      <c r="P11" s="70"/>
     </row>
     <row r="12" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="15"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="49"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="50"/>
       <c r="E12" s="19"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
@@ -3012,13 +3006,13 @@
       <c r="L12" s="20"/>
       <c r="M12" s="20"/>
       <c r="N12" s="21"/>
-      <c r="O12" s="58"/>
-      <c r="P12" s="59"/>
+      <c r="O12" s="69"/>
+      <c r="P12" s="70"/>
     </row>
     <row r="13" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="15"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="50"/>
       <c r="E13" s="19"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
@@ -3029,13 +3023,13 @@
       <c r="L13" s="20"/>
       <c r="M13" s="20"/>
       <c r="N13" s="21"/>
-      <c r="O13" s="58"/>
-      <c r="P13" s="59"/>
+      <c r="O13" s="69"/>
+      <c r="P13" s="70"/>
     </row>
     <row r="14" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="15"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="49"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="50"/>
       <c r="E14" s="19"/>
       <c r="F14" s="20"/>
       <c r="G14" s="20"/>
@@ -3046,13 +3040,13 @@
       <c r="L14" s="20"/>
       <c r="M14" s="20"/>
       <c r="N14" s="21"/>
-      <c r="O14" s="58"/>
-      <c r="P14" s="59"/>
+      <c r="O14" s="69"/>
+      <c r="P14" s="70"/>
     </row>
     <row r="15" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="15"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="49"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="50"/>
       <c r="E15" s="19"/>
       <c r="F15" s="20"/>
       <c r="G15" s="20"/>
@@ -3065,13 +3059,13 @@
       <c r="L15" s="20"/>
       <c r="M15" s="20"/>
       <c r="N15" s="21"/>
-      <c r="O15" s="58"/>
-      <c r="P15" s="59"/>
+      <c r="O15" s="69"/>
+      <c r="P15" s="70"/>
     </row>
     <row r="16" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="15"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="49"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="50"/>
       <c r="E16" s="19"/>
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
@@ -3082,13 +3076,13 @@
       <c r="L16" s="20"/>
       <c r="M16" s="20"/>
       <c r="N16" s="21"/>
-      <c r="O16" s="58"/>
-      <c r="P16" s="59"/>
+      <c r="O16" s="69"/>
+      <c r="P16" s="70"/>
     </row>
     <row r="17" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="15"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="50"/>
       <c r="E17" s="22"/>
       <c r="F17" s="23"/>
       <c r="G17" s="23"/>
@@ -3099,13 +3093,13 @@
       <c r="L17" s="23"/>
       <c r="M17" s="23"/>
       <c r="N17" s="24"/>
-      <c r="O17" s="58"/>
-      <c r="P17" s="59"/>
+      <c r="O17" s="69"/>
+      <c r="P17" s="70"/>
     </row>
     <row r="18" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="15"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="50"/>
       <c r="E18" s="11"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
@@ -3116,13 +3110,13 @@
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
       <c r="N18" s="12"/>
-      <c r="O18" s="58"/>
-      <c r="P18" s="59"/>
+      <c r="O18" s="69"/>
+      <c r="P18" s="70"/>
     </row>
     <row r="19" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="15"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="50"/>
       <c r="E19" s="11"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
@@ -3133,13 +3127,13 @@
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
       <c r="N19" s="12"/>
-      <c r="O19" s="58"/>
-      <c r="P19" s="59"/>
+      <c r="O19" s="69"/>
+      <c r="P19" s="70"/>
     </row>
     <row r="20" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="15"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="50"/>
       <c r="E20" s="11"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
@@ -3150,13 +3144,13 @@
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
       <c r="N20" s="12"/>
-      <c r="O20" s="58"/>
-      <c r="P20" s="59"/>
+      <c r="O20" s="69"/>
+      <c r="P20" s="70"/>
     </row>
     <row r="21" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="15"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="50"/>
       <c r="E21" s="11"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -3167,13 +3161,13 @@
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
       <c r="N21" s="12"/>
-      <c r="O21" s="58"/>
-      <c r="P21" s="59"/>
+      <c r="O21" s="69"/>
+      <c r="P21" s="70"/>
     </row>
     <row r="22" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="15"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="49"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="50"/>
       <c r="E22" s="11"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -3184,13 +3178,13 @@
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
       <c r="N22" s="12"/>
-      <c r="O22" s="58"/>
-      <c r="P22" s="59"/>
+      <c r="O22" s="69"/>
+      <c r="P22" s="70"/>
     </row>
     <row r="23" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="15"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="50"/>
       <c r="E23" s="11"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
@@ -3201,13 +3195,13 @@
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
       <c r="N23" s="12"/>
-      <c r="O23" s="58"/>
-      <c r="P23" s="59"/>
+      <c r="O23" s="69"/>
+      <c r="P23" s="70"/>
     </row>
     <row r="24" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="15"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="49"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="50"/>
       <c r="E24" s="11"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -3218,13 +3212,13 @@
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
       <c r="N24" s="12"/>
-      <c r="O24" s="58"/>
-      <c r="P24" s="59"/>
+      <c r="O24" s="69"/>
+      <c r="P24" s="70"/>
     </row>
     <row r="25" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="15"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="49"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="50"/>
       <c r="E25" s="11"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
@@ -3235,13 +3229,13 @@
       <c r="L25" s="9"/>
       <c r="M25" s="9"/>
       <c r="N25" s="12"/>
-      <c r="O25" s="58"/>
-      <c r="P25" s="59"/>
+      <c r="O25" s="69"/>
+      <c r="P25" s="70"/>
     </row>
     <row r="26" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="15"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="49"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="50"/>
       <c r="E26" s="11"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
@@ -3252,13 +3246,13 @@
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
       <c r="N26" s="12"/>
-      <c r="O26" s="58"/>
-      <c r="P26" s="59"/>
+      <c r="O26" s="69"/>
+      <c r="P26" s="70"/>
     </row>
     <row r="27" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="15"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="51"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="52"/>
       <c r="E27" s="4"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -3269,13 +3263,13 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="13"/>
-      <c r="O27" s="60"/>
-      <c r="P27" s="61"/>
+      <c r="O27" s="71"/>
+      <c r="P27" s="72"/>
     </row>
     <row r="28" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="15"/>
-      <c r="C28" s="52"/>
-      <c r="D28" s="53"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="48"/>
       <c r="E28" s="6"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -3286,13 +3280,13 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="10"/>
-      <c r="O28" s="62"/>
-      <c r="P28" s="63"/>
+      <c r="O28" s="53"/>
+      <c r="P28" s="54"/>
     </row>
     <row r="29" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="15"/>
-      <c r="C29" s="48"/>
-      <c r="D29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="50"/>
       <c r="E29" s="11"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
@@ -3303,13 +3297,13 @@
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
       <c r="N29" s="12"/>
-      <c r="O29" s="64"/>
-      <c r="P29" s="65"/>
+      <c r="O29" s="55"/>
+      <c r="P29" s="56"/>
     </row>
     <row r="30" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="15"/>
-      <c r="C30" s="48"/>
-      <c r="D30" s="49"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="50"/>
       <c r="E30" s="11"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
@@ -3320,13 +3314,13 @@
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
       <c r="N30" s="12"/>
-      <c r="O30" s="64"/>
-      <c r="P30" s="65"/>
+      <c r="O30" s="55"/>
+      <c r="P30" s="56"/>
     </row>
     <row r="31" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="15"/>
-      <c r="C31" s="48"/>
-      <c r="D31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="50"/>
       <c r="E31" s="11"/>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
@@ -3337,13 +3331,13 @@
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
       <c r="N31" s="12"/>
-      <c r="O31" s="64"/>
-      <c r="P31" s="65"/>
+      <c r="O31" s="55"/>
+      <c r="P31" s="56"/>
     </row>
     <row r="32" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="15"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="49"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="50"/>
       <c r="E32" s="11"/>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
@@ -3354,13 +3348,13 @@
       <c r="L32" s="9"/>
       <c r="M32" s="9"/>
       <c r="N32" s="12"/>
-      <c r="O32" s="64"/>
-      <c r="P32" s="65"/>
+      <c r="O32" s="55"/>
+      <c r="P32" s="56"/>
     </row>
     <row r="33" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="15"/>
-      <c r="C33" s="48"/>
-      <c r="D33" s="49"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="50"/>
       <c r="E33" s="11"/>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
@@ -3371,13 +3365,13 @@
       <c r="L33" s="9"/>
       <c r="M33" s="9"/>
       <c r="N33" s="12"/>
-      <c r="O33" s="64"/>
-      <c r="P33" s="65"/>
+      <c r="O33" s="55"/>
+      <c r="P33" s="56"/>
     </row>
     <row r="34" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="15"/>
-      <c r="C34" s="48"/>
-      <c r="D34" s="49"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="50"/>
       <c r="E34" s="11"/>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
@@ -3388,13 +3382,13 @@
       <c r="L34" s="9"/>
       <c r="M34" s="9"/>
       <c r="N34" s="12"/>
-      <c r="O34" s="64"/>
-      <c r="P34" s="65"/>
+      <c r="O34" s="55"/>
+      <c r="P34" s="56"/>
     </row>
     <row r="35" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="15"/>
-      <c r="C35" s="48"/>
-      <c r="D35" s="49"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="50"/>
       <c r="E35" s="11"/>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
@@ -3405,13 +3399,13 @@
       <c r="L35" s="9"/>
       <c r="M35" s="9"/>
       <c r="N35" s="12"/>
-      <c r="O35" s="64"/>
-      <c r="P35" s="65"/>
+      <c r="O35" s="55"/>
+      <c r="P35" s="56"/>
     </row>
     <row r="36" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="15"/>
-      <c r="C36" s="48"/>
-      <c r="D36" s="49"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="50"/>
       <c r="E36" s="11"/>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
@@ -3422,13 +3416,13 @@
       <c r="L36" s="9"/>
       <c r="M36" s="9"/>
       <c r="N36" s="12"/>
-      <c r="O36" s="64"/>
-      <c r="P36" s="65"/>
+      <c r="O36" s="55"/>
+      <c r="P36" s="56"/>
     </row>
     <row r="37" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="15"/>
-      <c r="C37" s="48"/>
-      <c r="D37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="50"/>
       <c r="E37" s="11"/>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
@@ -3439,13 +3433,13 @@
       <c r="L37" s="9"/>
       <c r="M37" s="9"/>
       <c r="N37" s="12"/>
-      <c r="O37" s="64"/>
-      <c r="P37" s="65"/>
+      <c r="O37" s="55"/>
+      <c r="P37" s="56"/>
     </row>
     <row r="38" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" s="15"/>
-      <c r="C38" s="50"/>
-      <c r="D38" s="51"/>
+      <c r="C38" s="51"/>
+      <c r="D38" s="52"/>
       <c r="E38" s="25"/>
       <c r="F38" s="26"/>
       <c r="G38" s="26"/>
@@ -3456,14 +3450,14 @@
       <c r="L38" s="26"/>
       <c r="M38" s="26"/>
       <c r="N38" s="27"/>
-      <c r="O38" s="66"/>
-      <c r="P38" s="67"/>
+      <c r="O38" s="57"/>
+      <c r="P38" s="58"/>
     </row>
     <row r="39" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39"/>
       <c r="B39"/>
-      <c r="C39" s="68"/>
-      <c r="D39" s="69"/>
+      <c r="C39" s="59"/>
+      <c r="D39" s="60"/>
       <c r="E39" s="29"/>
       <c r="F39" s="28"/>
       <c r="G39" s="28"/>
@@ -3474,8 +3468,8 @@
       <c r="L39" s="28"/>
       <c r="M39" s="28"/>
       <c r="N39" s="30"/>
-      <c r="O39" s="68"/>
-      <c r="P39" s="69"/>
+      <c r="O39" s="59"/>
+      <c r="P39" s="60"/>
       <c r="Q39"/>
       <c r="R39"/>
       <c r="S39"/>
@@ -3483,8 +3477,8 @@
     <row r="40" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40"/>
       <c r="B40"/>
-      <c r="C40" s="70"/>
-      <c r="D40" s="71"/>
+      <c r="C40" s="61"/>
+      <c r="D40" s="62"/>
       <c r="E40" s="29"/>
       <c r="F40" s="28"/>
       <c r="G40" s="28"/>
@@ -3495,8 +3489,8 @@
       <c r="L40" s="28"/>
       <c r="M40" s="28"/>
       <c r="N40" s="30"/>
-      <c r="O40" s="70"/>
-      <c r="P40" s="71"/>
+      <c r="O40" s="61"/>
+      <c r="P40" s="62"/>
       <c r="Q40"/>
       <c r="R40"/>
       <c r="S40"/>
@@ -3504,8 +3498,8 @@
     <row r="41" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41"/>
       <c r="B41"/>
-      <c r="C41" s="70"/>
-      <c r="D41" s="71"/>
+      <c r="C41" s="61"/>
+      <c r="D41" s="62"/>
       <c r="E41" s="29"/>
       <c r="F41" s="28"/>
       <c r="G41" s="28"/>
@@ -3516,8 +3510,8 @@
       <c r="L41" s="28"/>
       <c r="M41" s="28"/>
       <c r="N41" s="30"/>
-      <c r="O41" s="70"/>
-      <c r="P41" s="71"/>
+      <c r="O41" s="61"/>
+      <c r="P41" s="62"/>
       <c r="Q41"/>
       <c r="R41"/>
       <c r="S41"/>
@@ -3525,8 +3519,8 @@
     <row r="42" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42"/>
       <c r="B42"/>
-      <c r="C42" s="70"/>
-      <c r="D42" s="71"/>
+      <c r="C42" s="61"/>
+      <c r="D42" s="62"/>
       <c r="E42" s="29"/>
       <c r="F42" s="28"/>
       <c r="G42" s="28"/>
@@ -3537,8 +3531,8 @@
       <c r="L42" s="28"/>
       <c r="M42" s="28"/>
       <c r="N42" s="30"/>
-      <c r="O42" s="70"/>
-      <c r="P42" s="71"/>
+      <c r="O42" s="61"/>
+      <c r="P42" s="62"/>
       <c r="Q42"/>
       <c r="R42"/>
       <c r="S42"/>
@@ -3546,8 +3540,8 @@
     <row r="43" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43"/>
       <c r="B43"/>
-      <c r="C43" s="72"/>
-      <c r="D43" s="73"/>
+      <c r="C43" s="63"/>
+      <c r="D43" s="64"/>
       <c r="E43" s="29"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
@@ -3558,8 +3552,8 @@
       <c r="L43" s="28"/>
       <c r="M43" s="28"/>
       <c r="N43" s="30"/>
-      <c r="O43" s="72"/>
-      <c r="P43" s="73"/>
+      <c r="O43" s="63"/>
+      <c r="P43" s="64"/>
       <c r="Q43"/>
       <c r="R43"/>
       <c r="S43"/>
@@ -3692,11 +3686,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C28:D29"/>
-    <mergeCell ref="C30:D38"/>
-    <mergeCell ref="O28:P38"/>
-    <mergeCell ref="C39:D43"/>
-    <mergeCell ref="O39:P43"/>
     <mergeCell ref="C1:P1"/>
     <mergeCell ref="F2:K3"/>
     <mergeCell ref="N2:O2"/>
@@ -3706,6 +3695,11 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="O5:P6"/>
     <mergeCell ref="O7:P27"/>
+    <mergeCell ref="C28:D29"/>
+    <mergeCell ref="C30:D38"/>
+    <mergeCell ref="O28:P38"/>
+    <mergeCell ref="C39:D43"/>
+    <mergeCell ref="O39:P43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="35" orientation="portrait" r:id="rId1"/>
@@ -3752,84 +3746,84 @@
       <c r="C10" s="36"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="75" t="s">
+      <c r="A13" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="75"/>
-      <c r="C13" s="75" t="s">
+      <c r="B13" s="73"/>
+      <c r="C13" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="75"/>
-      <c r="E13" s="75" t="s">
+      <c r="D13" s="73"/>
+      <c r="E13" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="75" t="s">
+      <c r="F13" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="75"/>
-      <c r="H13" s="75" t="s">
+      <c r="G13" s="73"/>
+      <c r="H13" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="I13" s="75"/>
+      <c r="I13" s="73"/>
     </row>
     <row r="14" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="75"/>
-      <c r="B14" s="75"/>
-      <c r="C14" s="75"/>
-      <c r="D14" s="75"/>
-      <c r="E14" s="75"/>
-      <c r="F14" s="75"/>
-      <c r="G14" s="75"/>
-      <c r="H14" s="75"/>
-      <c r="I14" s="75"/>
+      <c r="A14" s="73"/>
+      <c r="B14" s="73"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73"/>
+      <c r="G14" s="73"/>
+      <c r="H14" s="73"/>
+      <c r="I14" s="73"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="75" t="s">
+      <c r="A15" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="75"/>
-      <c r="C15" s="75"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="75"/>
-      <c r="I15" s="75"/>
+      <c r="B15" s="73"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="73"/>
+      <c r="G15" s="73"/>
+      <c r="H15" s="73"/>
+      <c r="I15" s="73"/>
     </row>
     <row r="16" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="75"/>
-      <c r="B16" s="75"/>
-      <c r="C16" s="75"/>
-      <c r="D16" s="75"/>
-      <c r="E16" s="75"/>
-      <c r="F16" s="75"/>
-      <c r="G16" s="75"/>
-      <c r="H16" s="75"/>
-      <c r="I16" s="75"/>
+      <c r="A16" s="73"/>
+      <c r="B16" s="73"/>
+      <c r="C16" s="73"/>
+      <c r="D16" s="73"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="73"/>
+      <c r="G16" s="73"/>
+      <c r="H16" s="73"/>
+      <c r="I16" s="73"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="75" t="s">
+      <c r="A17" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="75"/>
-      <c r="C17" s="75"/>
-      <c r="D17" s="75"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="75"/>
-      <c r="I17" s="75"/>
+      <c r="B17" s="73"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="73"/>
+      <c r="H17" s="73"/>
+      <c r="I17" s="73"/>
     </row>
     <row r="18" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="75"/>
-      <c r="B18" s="75"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="75"/>
-      <c r="E18" s="75"/>
-      <c r="F18" s="75"/>
-      <c r="G18" s="75"/>
-      <c r="H18" s="75"/>
-      <c r="I18" s="75"/>
+      <c r="A18" s="73"/>
+      <c r="B18" s="73"/>
+      <c r="C18" s="73"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="73"/>
+      <c r="H18" s="73"/>
+      <c r="I18" s="73"/>
     </row>
     <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="37"/>
@@ -3837,12 +3831,12 @@
       <c r="C19" s="37"/>
       <c r="D19" s="37"/>
       <c r="E19" s="37"/>
-      <c r="F19" s="75" t="s">
+      <c r="F19" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="75"/>
-      <c r="H19" s="75"/>
-      <c r="I19" s="75"/>
+      <c r="G19" s="73"/>
+      <c r="H19" s="73"/>
+      <c r="I19" s="73"/>
     </row>
     <row r="20" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="37"/>
@@ -3850,106 +3844,106 @@
       <c r="C20" s="37"/>
       <c r="D20" s="37"/>
       <c r="E20" s="37"/>
-      <c r="F20" s="75"/>
-      <c r="G20" s="75"/>
-      <c r="H20" s="75"/>
-      <c r="I20" s="75"/>
+      <c r="F20" s="73"/>
+      <c r="G20" s="73"/>
+      <c r="H20" s="73"/>
+      <c r="I20" s="73"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="75" t="s">
+      <c r="A21" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="75"/>
-      <c r="C21" s="75"/>
-      <c r="D21" s="75"/>
-      <c r="E21" s="75"/>
-      <c r="F21" s="75"/>
-      <c r="G21" s="75"/>
-      <c r="H21" s="75"/>
-      <c r="I21" s="75"/>
+      <c r="B21" s="73"/>
+      <c r="C21" s="73"/>
+      <c r="D21" s="73"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="73"/>
+      <c r="G21" s="73"/>
+      <c r="H21" s="73"/>
+      <c r="I21" s="73"/>
     </row>
     <row r="22" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="75"/>
-      <c r="B22" s="75"/>
-      <c r="C22" s="75"/>
-      <c r="D22" s="75"/>
-      <c r="E22" s="75"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="75"/>
-      <c r="H22" s="75"/>
-      <c r="I22" s="75"/>
+      <c r="A22" s="73"/>
+      <c r="B22" s="73"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="73"/>
+      <c r="I22" s="73"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="75" t="s">
+      <c r="A23" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="75"/>
-      <c r="C23" s="75"/>
-      <c r="D23" s="75"/>
-      <c r="E23" s="75"/>
-      <c r="F23" s="75"/>
-      <c r="G23" s="75"/>
-      <c r="H23" s="75"/>
-      <c r="I23" s="75"/>
+      <c r="B23" s="73"/>
+      <c r="C23" s="73"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="73"/>
+      <c r="H23" s="73"/>
+      <c r="I23" s="73"/>
     </row>
     <row r="24" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="75"/>
-      <c r="B24" s="75"/>
-      <c r="C24" s="75"/>
-      <c r="D24" s="75"/>
-      <c r="E24" s="75"/>
-      <c r="F24" s="75"/>
-      <c r="G24" s="75"/>
-      <c r="H24" s="75"/>
-      <c r="I24" s="75"/>
+      <c r="A24" s="73"/>
+      <c r="B24" s="73"/>
+      <c r="C24" s="73"/>
+      <c r="D24" s="73"/>
+      <c r="E24" s="73"/>
+      <c r="F24" s="73"/>
+      <c r="G24" s="73"/>
+      <c r="H24" s="73"/>
+      <c r="I24" s="73"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="75" t="s">
+      <c r="A25" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="75"/>
-      <c r="C25" s="75"/>
-      <c r="D25" s="75"/>
-      <c r="E25" s="75"/>
-      <c r="F25" s="75"/>
-      <c r="G25" s="75"/>
-      <c r="H25" s="75"/>
-      <c r="I25" s="75"/>
+      <c r="B25" s="73"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="73"/>
+      <c r="H25" s="73"/>
+      <c r="I25" s="73"/>
     </row>
     <row r="26" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="75"/>
-      <c r="B26" s="75"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
-      <c r="F26" s="75"/>
-      <c r="G26" s="75"/>
-      <c r="H26" s="75"/>
-      <c r="I26" s="75"/>
+      <c r="A26" s="73"/>
+      <c r="B26" s="73"/>
+      <c r="C26" s="73"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="73"/>
+      <c r="F26" s="73"/>
+      <c r="G26" s="73"/>
+      <c r="H26" s="73"/>
+      <c r="I26" s="73"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="75" t="s">
+      <c r="A27" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="75"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="75"/>
-      <c r="H27" s="75"/>
-      <c r="I27" s="75"/>
+      <c r="B27" s="73"/>
+      <c r="C27" s="73"/>
+      <c r="D27" s="73"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="73"/>
+      <c r="H27" s="73"/>
+      <c r="I27" s="73"/>
     </row>
     <row r="28" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="75"/>
-      <c r="B28" s="75"/>
-      <c r="C28" s="75"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="75"/>
-      <c r="F28" s="75"/>
-      <c r="G28" s="75"/>
-      <c r="H28" s="75"/>
-      <c r="I28" s="75"/>
+      <c r="A28" s="73"/>
+      <c r="B28" s="73"/>
+      <c r="C28" s="73"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="73"/>
+      <c r="F28" s="73"/>
+      <c r="G28" s="73"/>
+      <c r="H28" s="73"/>
+      <c r="I28" s="73"/>
     </row>
     <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="38" t="s">
@@ -3960,6 +3954,34 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="A25:B26"/>
+    <mergeCell ref="C25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:G26"/>
+    <mergeCell ref="H25:I26"/>
+    <mergeCell ref="A27:B28"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:G28"/>
+    <mergeCell ref="H27:I28"/>
+    <mergeCell ref="F19:G20"/>
+    <mergeCell ref="H19:I20"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="C17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:G18"/>
+    <mergeCell ref="H17:I18"/>
+    <mergeCell ref="A21:B22"/>
+    <mergeCell ref="C21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:G22"/>
+    <mergeCell ref="H21:I22"/>
+    <mergeCell ref="A23:B24"/>
+    <mergeCell ref="C23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:G24"/>
+    <mergeCell ref="H23:I24"/>
     <mergeCell ref="F13:G14"/>
     <mergeCell ref="H13:I14"/>
     <mergeCell ref="A15:B16"/>
@@ -3970,34 +3992,6 @@
     <mergeCell ref="A13:B14"/>
     <mergeCell ref="C13:D14"/>
     <mergeCell ref="E13:E14"/>
-    <mergeCell ref="A23:B24"/>
-    <mergeCell ref="C23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:G24"/>
-    <mergeCell ref="H23:I24"/>
-    <mergeCell ref="A21:B22"/>
-    <mergeCell ref="C21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:G22"/>
-    <mergeCell ref="H21:I22"/>
-    <mergeCell ref="F19:G20"/>
-    <mergeCell ref="H19:I20"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="C17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:G18"/>
-    <mergeCell ref="H17:I18"/>
-    <mergeCell ref="H25:I26"/>
-    <mergeCell ref="A27:B28"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:G28"/>
-    <mergeCell ref="H27:I28"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="A25:B26"/>
-    <mergeCell ref="C25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:G26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4008,8 +4002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A016E41C-E536-466F-8BCC-D27E2EA7F174}">
   <dimension ref="A3:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4023,22 +4017,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="G3" s="76" t="s">
+      <c r="B3" s="75"/>
+      <c r="G3" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
     </row>
     <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G5" s="77" t="s">
+      <c r="G5" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
     </row>
     <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="40" t="s">
@@ -4046,37 +4040,37 @@
       </c>
       <c r="B6" s="42"/>
       <c r="C6" s="39"/>
-      <c r="G6" s="77"/>
-      <c r="H6" s="77"/>
-      <c r="I6" s="77"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="76"/>
     </row>
     <row r="7" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="42"/>
       <c r="C7" s="39"/>
-      <c r="G7" s="77"/>
-      <c r="H7" s="77"/>
-      <c r="I7" s="77"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="76"/>
     </row>
     <row r="8" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="42"/>
       <c r="C8" s="39"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="77"/>
-      <c r="I8" s="77"/>
+      <c r="G8" s="76"/>
+      <c r="H8" s="76"/>
+      <c r="I8" s="76"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B9" s="42"/>
       <c r="C9" s="39"/>
-      <c r="G9" s="77"/>
-      <c r="H9" s="77"/>
-      <c r="I9" s="77"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="76"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B10" s="42"/>
       <c r="C10" s="39"/>
-      <c r="G10" s="77"/>
-      <c r="H10" s="77"/>
-      <c r="I10" s="77"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="76"/>
     </row>
     <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
@@ -4084,9 +4078,9 @@
       </c>
       <c r="B11" s="42"/>
       <c r="C11" s="39"/>
-      <c r="G11" s="77"/>
-      <c r="H11" s="77"/>
-      <c r="I11" s="77"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="76"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B12" s="42"/>
@@ -4110,9 +4104,6 @@
       </c>
       <c r="B16" s="42"/>
       <c r="C16" s="39"/>
-      <c r="G16" s="43" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B17" s="42"/>
@@ -4137,14 +4128,12 @@
       <c r="B21" s="42"/>
       <c r="C21" s="39"/>
     </row>
-    <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B22" s="42"/>
       <c r="C22" s="39"/>
-      <c r="G22" s="76" t="s">
-        <v>31</v>
-      </c>
-      <c r="H22" s="76"/>
-      <c r="I22" s="76"/>
+      <c r="G22" s="77" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B23" s="42"/>
@@ -4153,12 +4142,6 @@
     <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B24" s="42"/>
       <c r="C24" s="39"/>
-      <c r="G24" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="I24" s="31" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B25" s="42"/>
@@ -4175,9 +4158,14 @@
       <c r="B27" s="42"/>
       <c r="C27" s="39"/>
     </row>
-    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="B28" s="42"/>
       <c r="C28" s="39"/>
+      <c r="G28" s="75" t="s">
+        <v>31</v>
+      </c>
+      <c r="H28" s="75"/>
+      <c r="I28" s="75"/>
     </row>
     <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B29" s="42"/>
@@ -4300,7 +4288,7 @@
   <mergeCells count="4">
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G28:I28"/>
     <mergeCell ref="G5:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
brought back bloody and green condemn
</commit_message>
<xml_diff>
--- a/CustomLabelPrinter/src/paperwork/recap.xlsx
+++ b/CustomLabelPrinter/src/paperwork/recap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\pdgwinterm7\git\repository\CustomLabelPrinter\src\paperwork\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdphu\git\customlabelprinter\CustomLabelPrinter\src\paperwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A67FC0-8E5D-414D-9A8F-17728A6851D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7094907F-63B8-41FB-80D0-7BFDC8CA68F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="10740" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8925" yWindow="825" windowWidth="25740" windowHeight="15975" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BREAST" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t>Total Tender Condemned</t>
+  </si>
+  <si>
+    <t>Blood</t>
+  </si>
+  <si>
+    <t>Green</t>
   </si>
 </sst>
 </file>
@@ -618,6 +624,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -630,23 +637,47 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -684,43 +715,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1018,54 +1024,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="35.25" x14ac:dyDescent="0.25">
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="43"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
     </row>
     <row r="2" spans="2:19" ht="27.75" x14ac:dyDescent="0.4">
       <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="44"/>
-      <c r="F2" s="45" t="s">
+      <c r="E2" s="45"/>
+      <c r="F2" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
       <c r="L2" s="7"/>
       <c r="M2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
       <c r="P2" s="7"/>
     </row>
     <row r="3" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
     </row>
     <row r="4" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E4" s="8">
@@ -1098,10 +1104,10 @@
       <c r="N4" s="8">
         <v>26</v>
       </c>
-      <c r="O4" s="46" t="s">
+      <c r="O4" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="46"/>
+      <c r="P4" s="47"/>
       <c r="R4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1902,57 +1908,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="35.25" x14ac:dyDescent="0.25">
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="43"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
     </row>
     <row r="2" spans="2:19" ht="27.75" x14ac:dyDescent="0.4">
       <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="44"/>
-      <c r="F2" s="45" t="s">
+      <c r="E2" s="45"/>
+      <c r="F2" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
       <c r="L2" s="7"/>
       <c r="M2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
       <c r="P2" s="7"/>
       <c r="S2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
     </row>
     <row r="4" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E4" s="8">
@@ -1985,10 +1991,10 @@
       <c r="N4" s="8">
         <v>26</v>
       </c>
-      <c r="O4" s="46" t="s">
+      <c r="O4" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="46"/>
+      <c r="P4" s="47"/>
     </row>
     <row r="5" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="15"/>
@@ -2783,54 +2789,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="35.25" x14ac:dyDescent="0.25">
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="43"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
     </row>
     <row r="2" spans="2:19" ht="27.75" x14ac:dyDescent="0.4">
       <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="44"/>
-      <c r="F2" s="45" t="s">
+      <c r="E2" s="45"/>
+      <c r="F2" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
       <c r="L2" s="7"/>
       <c r="M2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
       <c r="P2" s="7"/>
     </row>
     <row r="3" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
     </row>
     <row r="4" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E4" s="8">
@@ -2863,20 +2869,20 @@
       <c r="N4" s="8">
         <v>26</v>
       </c>
-      <c r="O4" s="46" t="s">
+      <c r="O4" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="46"/>
+      <c r="P4" s="47"/>
       <c r="S4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="15"/>
-      <c r="C5" s="47">
+      <c r="C5" s="52">
         <v>22486</v>
       </c>
-      <c r="D5" s="48"/>
+      <c r="D5" s="53"/>
       <c r="E5" s="16"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
@@ -2887,13 +2893,13 @@
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
       <c r="N5" s="18"/>
-      <c r="O5" s="65"/>
-      <c r="P5" s="66"/>
+      <c r="O5" s="54"/>
+      <c r="P5" s="55"/>
     </row>
     <row r="6" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="15"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="50"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="49"/>
       <c r="E6" s="19"/>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
@@ -2904,13 +2910,13 @@
       <c r="L6" s="20"/>
       <c r="M6" s="20"/>
       <c r="N6" s="21"/>
-      <c r="O6" s="67"/>
-      <c r="P6" s="68"/>
+      <c r="O6" s="56"/>
+      <c r="P6" s="57"/>
     </row>
     <row r="7" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="15"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="50"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="49"/>
       <c r="E7" s="19"/>
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
@@ -2921,13 +2927,13 @@
       <c r="L7" s="20"/>
       <c r="M7" s="20"/>
       <c r="N7" s="21"/>
-      <c r="O7" s="69"/>
-      <c r="P7" s="70"/>
+      <c r="O7" s="58"/>
+      <c r="P7" s="59"/>
     </row>
     <row r="8" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="15"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="50"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="49"/>
       <c r="E8" s="19"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
@@ -2938,13 +2944,13 @@
       <c r="L8" s="20"/>
       <c r="M8" s="20"/>
       <c r="N8" s="21"/>
-      <c r="O8" s="69"/>
-      <c r="P8" s="70"/>
+      <c r="O8" s="58"/>
+      <c r="P8" s="59"/>
     </row>
     <row r="9" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="15"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="50"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="49"/>
       <c r="E9" s="19"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
@@ -2955,13 +2961,13 @@
       <c r="L9" s="20"/>
       <c r="M9" s="20"/>
       <c r="N9" s="21"/>
-      <c r="O9" s="69"/>
-      <c r="P9" s="70"/>
+      <c r="O9" s="58"/>
+      <c r="P9" s="59"/>
     </row>
     <row r="10" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="15"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="50"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="49"/>
       <c r="E10" s="19"/>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
@@ -2972,13 +2978,13 @@
       <c r="L10" s="20"/>
       <c r="M10" s="20"/>
       <c r="N10" s="21"/>
-      <c r="O10" s="69"/>
-      <c r="P10" s="70"/>
+      <c r="O10" s="58"/>
+      <c r="P10" s="59"/>
     </row>
     <row r="11" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="15"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="50"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="49"/>
       <c r="E11" s="19"/>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
@@ -2989,13 +2995,13 @@
       <c r="L11" s="20"/>
       <c r="M11" s="20"/>
       <c r="N11" s="21"/>
-      <c r="O11" s="69"/>
-      <c r="P11" s="70"/>
+      <c r="O11" s="58"/>
+      <c r="P11" s="59"/>
     </row>
     <row r="12" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="15"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="50"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="49"/>
       <c r="E12" s="19"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
@@ -3006,13 +3012,13 @@
       <c r="L12" s="20"/>
       <c r="M12" s="20"/>
       <c r="N12" s="21"/>
-      <c r="O12" s="69"/>
-      <c r="P12" s="70"/>
+      <c r="O12" s="58"/>
+      <c r="P12" s="59"/>
     </row>
     <row r="13" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="15"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="50"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="49"/>
       <c r="E13" s="19"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
@@ -3023,13 +3029,13 @@
       <c r="L13" s="20"/>
       <c r="M13" s="20"/>
       <c r="N13" s="21"/>
-      <c r="O13" s="69"/>
-      <c r="P13" s="70"/>
+      <c r="O13" s="58"/>
+      <c r="P13" s="59"/>
     </row>
     <row r="14" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="15"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="50"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="49"/>
       <c r="E14" s="19"/>
       <c r="F14" s="20"/>
       <c r="G14" s="20"/>
@@ -3040,13 +3046,13 @@
       <c r="L14" s="20"/>
       <c r="M14" s="20"/>
       <c r="N14" s="21"/>
-      <c r="O14" s="69"/>
-      <c r="P14" s="70"/>
+      <c r="O14" s="58"/>
+      <c r="P14" s="59"/>
     </row>
     <row r="15" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="15"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="50"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="49"/>
       <c r="E15" s="19"/>
       <c r="F15" s="20"/>
       <c r="G15" s="20"/>
@@ -3059,13 +3065,13 @@
       <c r="L15" s="20"/>
       <c r="M15" s="20"/>
       <c r="N15" s="21"/>
-      <c r="O15" s="69"/>
-      <c r="P15" s="70"/>
+      <c r="O15" s="58"/>
+      <c r="P15" s="59"/>
     </row>
     <row r="16" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="15"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="50"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="49"/>
       <c r="E16" s="19"/>
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
@@ -3076,13 +3082,13 @@
       <c r="L16" s="20"/>
       <c r="M16" s="20"/>
       <c r="N16" s="21"/>
-      <c r="O16" s="69"/>
-      <c r="P16" s="70"/>
+      <c r="O16" s="58"/>
+      <c r="P16" s="59"/>
     </row>
     <row r="17" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="15"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="50"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="49"/>
       <c r="E17" s="22"/>
       <c r="F17" s="23"/>
       <c r="G17" s="23"/>
@@ -3093,13 +3099,13 @@
       <c r="L17" s="23"/>
       <c r="M17" s="23"/>
       <c r="N17" s="24"/>
-      <c r="O17" s="69"/>
-      <c r="P17" s="70"/>
+      <c r="O17" s="58"/>
+      <c r="P17" s="59"/>
     </row>
     <row r="18" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="15"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="50"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="49"/>
       <c r="E18" s="11"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
@@ -3110,13 +3116,13 @@
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
       <c r="N18" s="12"/>
-      <c r="O18" s="69"/>
-      <c r="P18" s="70"/>
+      <c r="O18" s="58"/>
+      <c r="P18" s="59"/>
     </row>
     <row r="19" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="15"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="50"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="49"/>
       <c r="E19" s="11"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
@@ -3127,13 +3133,13 @@
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
       <c r="N19" s="12"/>
-      <c r="O19" s="69"/>
-      <c r="P19" s="70"/>
+      <c r="O19" s="58"/>
+      <c r="P19" s="59"/>
     </row>
     <row r="20" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="15"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="50"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="49"/>
       <c r="E20" s="11"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
@@ -3144,13 +3150,13 @@
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
       <c r="N20" s="12"/>
-      <c r="O20" s="69"/>
-      <c r="P20" s="70"/>
+      <c r="O20" s="58"/>
+      <c r="P20" s="59"/>
     </row>
     <row r="21" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="15"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="50"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="49"/>
       <c r="E21" s="11"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -3161,13 +3167,13 @@
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
       <c r="N21" s="12"/>
-      <c r="O21" s="69"/>
-      <c r="P21" s="70"/>
+      <c r="O21" s="58"/>
+      <c r="P21" s="59"/>
     </row>
     <row r="22" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="15"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="50"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="49"/>
       <c r="E22" s="11"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -3178,13 +3184,13 @@
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
       <c r="N22" s="12"/>
-      <c r="O22" s="69"/>
-      <c r="P22" s="70"/>
+      <c r="O22" s="58"/>
+      <c r="P22" s="59"/>
     </row>
     <row r="23" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="15"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="50"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="49"/>
       <c r="E23" s="11"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
@@ -3195,13 +3201,13 @@
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
       <c r="N23" s="12"/>
-      <c r="O23" s="69"/>
-      <c r="P23" s="70"/>
+      <c r="O23" s="58"/>
+      <c r="P23" s="59"/>
     </row>
     <row r="24" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="15"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="50"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="49"/>
       <c r="E24" s="11"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -3212,13 +3218,13 @@
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
       <c r="N24" s="12"/>
-      <c r="O24" s="69"/>
-      <c r="P24" s="70"/>
+      <c r="O24" s="58"/>
+      <c r="P24" s="59"/>
     </row>
     <row r="25" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="15"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="50"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="49"/>
       <c r="E25" s="11"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
@@ -3229,13 +3235,13 @@
       <c r="L25" s="9"/>
       <c r="M25" s="9"/>
       <c r="N25" s="12"/>
-      <c r="O25" s="69"/>
-      <c r="P25" s="70"/>
+      <c r="O25" s="58"/>
+      <c r="P25" s="59"/>
     </row>
     <row r="26" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="15"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="50"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="49"/>
       <c r="E26" s="11"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
@@ -3246,13 +3252,13 @@
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
       <c r="N26" s="12"/>
-      <c r="O26" s="69"/>
-      <c r="P26" s="70"/>
+      <c r="O26" s="58"/>
+      <c r="P26" s="59"/>
     </row>
     <row r="27" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="15"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="52"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="51"/>
       <c r="E27" s="4"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -3263,13 +3269,13 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="13"/>
-      <c r="O27" s="71"/>
-      <c r="P27" s="72"/>
+      <c r="O27" s="60"/>
+      <c r="P27" s="61"/>
     </row>
     <row r="28" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="15"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="48"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="53"/>
       <c r="E28" s="6"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -3280,13 +3286,13 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="10"/>
-      <c r="O28" s="53"/>
-      <c r="P28" s="54"/>
+      <c r="O28" s="62"/>
+      <c r="P28" s="63"/>
     </row>
     <row r="29" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="15"/>
-      <c r="C29" s="49"/>
-      <c r="D29" s="50"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="49"/>
       <c r="E29" s="11"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
@@ -3297,13 +3303,13 @@
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
       <c r="N29" s="12"/>
-      <c r="O29" s="55"/>
-      <c r="P29" s="56"/>
+      <c r="O29" s="64"/>
+      <c r="P29" s="65"/>
     </row>
     <row r="30" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="15"/>
-      <c r="C30" s="49"/>
-      <c r="D30" s="50"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="49"/>
       <c r="E30" s="11"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
@@ -3314,13 +3320,13 @@
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
       <c r="N30" s="12"/>
-      <c r="O30" s="55"/>
-      <c r="P30" s="56"/>
+      <c r="O30" s="64"/>
+      <c r="P30" s="65"/>
     </row>
     <row r="31" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="15"/>
-      <c r="C31" s="49"/>
-      <c r="D31" s="50"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="49"/>
       <c r="E31" s="11"/>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
@@ -3331,13 +3337,13 @@
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
       <c r="N31" s="12"/>
-      <c r="O31" s="55"/>
-      <c r="P31" s="56"/>
+      <c r="O31" s="64"/>
+      <c r="P31" s="65"/>
     </row>
     <row r="32" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="15"/>
-      <c r="C32" s="49"/>
-      <c r="D32" s="50"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="49"/>
       <c r="E32" s="11"/>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
@@ -3348,13 +3354,13 @@
       <c r="L32" s="9"/>
       <c r="M32" s="9"/>
       <c r="N32" s="12"/>
-      <c r="O32" s="55"/>
-      <c r="P32" s="56"/>
+      <c r="O32" s="64"/>
+      <c r="P32" s="65"/>
     </row>
     <row r="33" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="15"/>
-      <c r="C33" s="49"/>
-      <c r="D33" s="50"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="49"/>
       <c r="E33" s="11"/>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
@@ -3365,13 +3371,13 @@
       <c r="L33" s="9"/>
       <c r="M33" s="9"/>
       <c r="N33" s="12"/>
-      <c r="O33" s="55"/>
-      <c r="P33" s="56"/>
+      <c r="O33" s="64"/>
+      <c r="P33" s="65"/>
     </row>
     <row r="34" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="15"/>
-      <c r="C34" s="49"/>
-      <c r="D34" s="50"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="49"/>
       <c r="E34" s="11"/>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
@@ -3382,13 +3388,13 @@
       <c r="L34" s="9"/>
       <c r="M34" s="9"/>
       <c r="N34" s="12"/>
-      <c r="O34" s="55"/>
-      <c r="P34" s="56"/>
+      <c r="O34" s="64"/>
+      <c r="P34" s="65"/>
     </row>
     <row r="35" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="15"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="50"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="49"/>
       <c r="E35" s="11"/>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
@@ -3399,13 +3405,13 @@
       <c r="L35" s="9"/>
       <c r="M35" s="9"/>
       <c r="N35" s="12"/>
-      <c r="O35" s="55"/>
-      <c r="P35" s="56"/>
+      <c r="O35" s="64"/>
+      <c r="P35" s="65"/>
     </row>
     <row r="36" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="15"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="50"/>
+      <c r="C36" s="48"/>
+      <c r="D36" s="49"/>
       <c r="E36" s="11"/>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
@@ -3416,13 +3422,13 @@
       <c r="L36" s="9"/>
       <c r="M36" s="9"/>
       <c r="N36" s="12"/>
-      <c r="O36" s="55"/>
-      <c r="P36" s="56"/>
+      <c r="O36" s="64"/>
+      <c r="P36" s="65"/>
     </row>
     <row r="37" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="15"/>
-      <c r="C37" s="49"/>
-      <c r="D37" s="50"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="49"/>
       <c r="E37" s="11"/>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
@@ -3433,13 +3439,13 @@
       <c r="L37" s="9"/>
       <c r="M37" s="9"/>
       <c r="N37" s="12"/>
-      <c r="O37" s="55"/>
-      <c r="P37" s="56"/>
+      <c r="O37" s="64"/>
+      <c r="P37" s="65"/>
     </row>
     <row r="38" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" s="15"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="52"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="51"/>
       <c r="E38" s="25"/>
       <c r="F38" s="26"/>
       <c r="G38" s="26"/>
@@ -3450,14 +3456,14 @@
       <c r="L38" s="26"/>
       <c r="M38" s="26"/>
       <c r="N38" s="27"/>
-      <c r="O38" s="57"/>
-      <c r="P38" s="58"/>
+      <c r="O38" s="66"/>
+      <c r="P38" s="67"/>
     </row>
     <row r="39" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39"/>
       <c r="B39"/>
-      <c r="C39" s="59"/>
-      <c r="D39" s="60"/>
+      <c r="C39" s="68"/>
+      <c r="D39" s="69"/>
       <c r="E39" s="29"/>
       <c r="F39" s="28"/>
       <c r="G39" s="28"/>
@@ -3468,8 +3474,8 @@
       <c r="L39" s="28"/>
       <c r="M39" s="28"/>
       <c r="N39" s="30"/>
-      <c r="O39" s="59"/>
-      <c r="P39" s="60"/>
+      <c r="O39" s="68"/>
+      <c r="P39" s="69"/>
       <c r="Q39"/>
       <c r="R39"/>
       <c r="S39"/>
@@ -3477,8 +3483,8 @@
     <row r="40" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40"/>
       <c r="B40"/>
-      <c r="C40" s="61"/>
-      <c r="D40" s="62"/>
+      <c r="C40" s="70"/>
+      <c r="D40" s="71"/>
       <c r="E40" s="29"/>
       <c r="F40" s="28"/>
       <c r="G40" s="28"/>
@@ -3489,8 +3495,8 @@
       <c r="L40" s="28"/>
       <c r="M40" s="28"/>
       <c r="N40" s="30"/>
-      <c r="O40" s="61"/>
-      <c r="P40" s="62"/>
+      <c r="O40" s="70"/>
+      <c r="P40" s="71"/>
       <c r="Q40"/>
       <c r="R40"/>
       <c r="S40"/>
@@ -3498,8 +3504,8 @@
     <row r="41" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41"/>
       <c r="B41"/>
-      <c r="C41" s="61"/>
-      <c r="D41" s="62"/>
+      <c r="C41" s="70"/>
+      <c r="D41" s="71"/>
       <c r="E41" s="29"/>
       <c r="F41" s="28"/>
       <c r="G41" s="28"/>
@@ -3510,8 +3516,8 @@
       <c r="L41" s="28"/>
       <c r="M41" s="28"/>
       <c r="N41" s="30"/>
-      <c r="O41" s="61"/>
-      <c r="P41" s="62"/>
+      <c r="O41" s="70"/>
+      <c r="P41" s="71"/>
       <c r="Q41"/>
       <c r="R41"/>
       <c r="S41"/>
@@ -3519,8 +3525,8 @@
     <row r="42" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42"/>
       <c r="B42"/>
-      <c r="C42" s="61"/>
-      <c r="D42" s="62"/>
+      <c r="C42" s="70"/>
+      <c r="D42" s="71"/>
       <c r="E42" s="29"/>
       <c r="F42" s="28"/>
       <c r="G42" s="28"/>
@@ -3531,8 +3537,8 @@
       <c r="L42" s="28"/>
       <c r="M42" s="28"/>
       <c r="N42" s="30"/>
-      <c r="O42" s="61"/>
-      <c r="P42" s="62"/>
+      <c r="O42" s="70"/>
+      <c r="P42" s="71"/>
       <c r="Q42"/>
       <c r="R42"/>
       <c r="S42"/>
@@ -3540,8 +3546,8 @@
     <row r="43" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43"/>
       <c r="B43"/>
-      <c r="C43" s="63"/>
-      <c r="D43" s="64"/>
+      <c r="C43" s="72"/>
+      <c r="D43" s="73"/>
       <c r="E43" s="29"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
@@ -3552,8 +3558,8 @@
       <c r="L43" s="28"/>
       <c r="M43" s="28"/>
       <c r="N43" s="30"/>
-      <c r="O43" s="63"/>
-      <c r="P43" s="64"/>
+      <c r="O43" s="72"/>
+      <c r="P43" s="73"/>
       <c r="Q43"/>
       <c r="R43"/>
       <c r="S43"/>
@@ -3686,6 +3692,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C28:D29"/>
+    <mergeCell ref="C30:D38"/>
+    <mergeCell ref="O28:P38"/>
+    <mergeCell ref="C39:D43"/>
+    <mergeCell ref="O39:P43"/>
     <mergeCell ref="C1:P1"/>
     <mergeCell ref="F2:K3"/>
     <mergeCell ref="N2:O2"/>
@@ -3695,11 +3706,6 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="O5:P6"/>
     <mergeCell ref="O7:P27"/>
-    <mergeCell ref="C28:D29"/>
-    <mergeCell ref="C30:D38"/>
-    <mergeCell ref="O28:P38"/>
-    <mergeCell ref="C39:D43"/>
-    <mergeCell ref="O39:P43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="35" orientation="portrait" r:id="rId1"/>
@@ -3746,84 +3752,84 @@
       <c r="C10" s="36"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="73" t="s">
+      <c r="A13" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="73"/>
-      <c r="C13" s="73" t="s">
+      <c r="B13" s="75"/>
+      <c r="C13" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73" t="s">
+      <c r="D13" s="75"/>
+      <c r="E13" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="73" t="s">
+      <c r="F13" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="73"/>
-      <c r="H13" s="73" t="s">
+      <c r="G13" s="75"/>
+      <c r="H13" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="I13" s="73"/>
+      <c r="I13" s="75"/>
     </row>
     <row r="14" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="73"/>
-      <c r="B14" s="73"/>
-      <c r="C14" s="73"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="73"/>
-      <c r="I14" s="73"/>
+      <c r="A14" s="75"/>
+      <c r="B14" s="75"/>
+      <c r="C14" s="75"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="75"/>
+      <c r="F14" s="75"/>
+      <c r="G14" s="75"/>
+      <c r="H14" s="75"/>
+      <c r="I14" s="75"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="73" t="s">
+      <c r="A15" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="73"/>
-      <c r="C15" s="73"/>
-      <c r="D15" s="73"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="73"/>
-      <c r="G15" s="73"/>
-      <c r="H15" s="73"/>
-      <c r="I15" s="73"/>
+      <c r="B15" s="75"/>
+      <c r="C15" s="75"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="75"/>
+      <c r="I15" s="75"/>
     </row>
     <row r="16" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="73"/>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="73"/>
-      <c r="H16" s="73"/>
-      <c r="I16" s="73"/>
+      <c r="A16" s="75"/>
+      <c r="B16" s="75"/>
+      <c r="C16" s="75"/>
+      <c r="D16" s="75"/>
+      <c r="E16" s="75"/>
+      <c r="F16" s="75"/>
+      <c r="G16" s="75"/>
+      <c r="H16" s="75"/>
+      <c r="I16" s="75"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="73" t="s">
+      <c r="A17" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="73"/>
-      <c r="C17" s="73"/>
-      <c r="D17" s="73"/>
-      <c r="E17" s="73"/>
-      <c r="F17" s="73"/>
-      <c r="G17" s="73"/>
-      <c r="H17" s="73"/>
-      <c r="I17" s="73"/>
+      <c r="B17" s="75"/>
+      <c r="C17" s="75"/>
+      <c r="D17" s="75"/>
+      <c r="E17" s="75"/>
+      <c r="F17" s="75"/>
+      <c r="G17" s="75"/>
+      <c r="H17" s="75"/>
+      <c r="I17" s="75"/>
     </row>
     <row r="18" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="73"/>
-      <c r="B18" s="73"/>
-      <c r="C18" s="73"/>
-      <c r="D18" s="73"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="73"/>
-      <c r="H18" s="73"/>
-      <c r="I18" s="73"/>
+      <c r="A18" s="75"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="75"/>
+      <c r="D18" s="75"/>
+      <c r="E18" s="75"/>
+      <c r="F18" s="75"/>
+      <c r="G18" s="75"/>
+      <c r="H18" s="75"/>
+      <c r="I18" s="75"/>
     </row>
     <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="37"/>
@@ -3831,12 +3837,12 @@
       <c r="C19" s="37"/>
       <c r="D19" s="37"/>
       <c r="E19" s="37"/>
-      <c r="F19" s="73" t="s">
+      <c r="F19" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="73"/>
-      <c r="H19" s="73"/>
-      <c r="I19" s="73"/>
+      <c r="G19" s="75"/>
+      <c r="H19" s="75"/>
+      <c r="I19" s="75"/>
     </row>
     <row r="20" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="37"/>
@@ -3844,106 +3850,106 @@
       <c r="C20" s="37"/>
       <c r="D20" s="37"/>
       <c r="E20" s="37"/>
-      <c r="F20" s="73"/>
-      <c r="G20" s="73"/>
-      <c r="H20" s="73"/>
-      <c r="I20" s="73"/>
+      <c r="F20" s="75"/>
+      <c r="G20" s="75"/>
+      <c r="H20" s="75"/>
+      <c r="I20" s="75"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="73" t="s">
+      <c r="A21" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="73"/>
-      <c r="C21" s="73"/>
-      <c r="D21" s="73"/>
-      <c r="E21" s="73"/>
-      <c r="F21" s="73"/>
-      <c r="G21" s="73"/>
-      <c r="H21" s="73"/>
-      <c r="I21" s="73"/>
+      <c r="B21" s="75"/>
+      <c r="C21" s="75"/>
+      <c r="D21" s="75"/>
+      <c r="E21" s="75"/>
+      <c r="F21" s="75"/>
+      <c r="G21" s="75"/>
+      <c r="H21" s="75"/>
+      <c r="I21" s="75"/>
     </row>
     <row r="22" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="73"/>
-      <c r="B22" s="73"/>
-      <c r="C22" s="73"/>
-      <c r="D22" s="73"/>
-      <c r="E22" s="73"/>
-      <c r="F22" s="73"/>
-      <c r="G22" s="73"/>
-      <c r="H22" s="73"/>
-      <c r="I22" s="73"/>
+      <c r="A22" s="75"/>
+      <c r="B22" s="75"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="75"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="75"/>
+      <c r="I22" s="75"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="73" t="s">
+      <c r="A23" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="73"/>
-      <c r="C23" s="73"/>
-      <c r="D23" s="73"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="73"/>
-      <c r="H23" s="73"/>
-      <c r="I23" s="73"/>
+      <c r="B23" s="75"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="75"/>
+      <c r="I23" s="75"/>
     </row>
     <row r="24" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="73"/>
-      <c r="B24" s="73"/>
-      <c r="C24" s="73"/>
-      <c r="D24" s="73"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="73"/>
-      <c r="G24" s="73"/>
-      <c r="H24" s="73"/>
-      <c r="I24" s="73"/>
+      <c r="A24" s="75"/>
+      <c r="B24" s="75"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="75"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="75"/>
+      <c r="I24" s="75"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="73" t="s">
+      <c r="A25" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="73"/>
-      <c r="C25" s="73"/>
-      <c r="D25" s="73"/>
-      <c r="E25" s="73"/>
-      <c r="F25" s="73"/>
-      <c r="G25" s="73"/>
-      <c r="H25" s="73"/>
-      <c r="I25" s="73"/>
+      <c r="B25" s="75"/>
+      <c r="C25" s="75"/>
+      <c r="D25" s="75"/>
+      <c r="E25" s="75"/>
+      <c r="F25" s="75"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="75"/>
+      <c r="I25" s="75"/>
     </row>
     <row r="26" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="73"/>
-      <c r="B26" s="73"/>
-      <c r="C26" s="73"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="73"/>
-      <c r="F26" s="73"/>
-      <c r="G26" s="73"/>
-      <c r="H26" s="73"/>
-      <c r="I26" s="73"/>
+      <c r="A26" s="75"/>
+      <c r="B26" s="75"/>
+      <c r="C26" s="75"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="75"/>
+      <c r="F26" s="75"/>
+      <c r="G26" s="75"/>
+      <c r="H26" s="75"/>
+      <c r="I26" s="75"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="73" t="s">
+      <c r="A27" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="73"/>
-      <c r="C27" s="73"/>
-      <c r="D27" s="73"/>
-      <c r="E27" s="73"/>
-      <c r="F27" s="73"/>
-      <c r="G27" s="73"/>
-      <c r="H27" s="73"/>
-      <c r="I27" s="73"/>
+      <c r="B27" s="75"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="75"/>
+      <c r="F27" s="75"/>
+      <c r="G27" s="75"/>
+      <c r="H27" s="75"/>
+      <c r="I27" s="75"/>
     </row>
     <row r="28" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="73"/>
-      <c r="B28" s="73"/>
-      <c r="C28" s="73"/>
-      <c r="D28" s="73"/>
-      <c r="E28" s="73"/>
-      <c r="F28" s="73"/>
-      <c r="G28" s="73"/>
-      <c r="H28" s="73"/>
-      <c r="I28" s="73"/>
+      <c r="A28" s="75"/>
+      <c r="B28" s="75"/>
+      <c r="C28" s="75"/>
+      <c r="D28" s="75"/>
+      <c r="E28" s="75"/>
+      <c r="F28" s="75"/>
+      <c r="G28" s="75"/>
+      <c r="H28" s="75"/>
+      <c r="I28" s="75"/>
     </row>
     <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="38" t="s">
@@ -3954,34 +3960,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="A25:B26"/>
-    <mergeCell ref="C25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:G26"/>
-    <mergeCell ref="H25:I26"/>
-    <mergeCell ref="A27:B28"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:G28"/>
-    <mergeCell ref="H27:I28"/>
-    <mergeCell ref="F19:G20"/>
-    <mergeCell ref="H19:I20"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="C17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:G18"/>
-    <mergeCell ref="H17:I18"/>
-    <mergeCell ref="A21:B22"/>
-    <mergeCell ref="C21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:G22"/>
-    <mergeCell ref="H21:I22"/>
-    <mergeCell ref="A23:B24"/>
-    <mergeCell ref="C23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:G24"/>
-    <mergeCell ref="H23:I24"/>
     <mergeCell ref="F13:G14"/>
     <mergeCell ref="H13:I14"/>
     <mergeCell ref="A15:B16"/>
@@ -3992,6 +3970,34 @@
     <mergeCell ref="A13:B14"/>
     <mergeCell ref="C13:D14"/>
     <mergeCell ref="E13:E14"/>
+    <mergeCell ref="A23:B24"/>
+    <mergeCell ref="C23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:G24"/>
+    <mergeCell ref="H23:I24"/>
+    <mergeCell ref="A21:B22"/>
+    <mergeCell ref="C21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:G22"/>
+    <mergeCell ref="H21:I22"/>
+    <mergeCell ref="F19:G20"/>
+    <mergeCell ref="H19:I20"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="C17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:G18"/>
+    <mergeCell ref="H17:I18"/>
+    <mergeCell ref="H25:I26"/>
+    <mergeCell ref="A27:B28"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:G28"/>
+    <mergeCell ref="H27:I28"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="A25:B26"/>
+    <mergeCell ref="C25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:G26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4002,8 +4008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A016E41C-E536-466F-8BCC-D27E2EA7F174}">
   <dimension ref="A3:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4017,22 +4023,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="75"/>
-      <c r="G3" s="75" t="s">
+      <c r="B3" s="76"/>
+      <c r="G3" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
     </row>
     <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G5" s="76" t="s">
+      <c r="G5" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="76"/>
-      <c r="I5" s="76"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
     </row>
     <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="40" t="s">
@@ -4040,37 +4046,37 @@
       </c>
       <c r="B6" s="42"/>
       <c r="C6" s="39"/>
-      <c r="G6" s="76"/>
-      <c r="H6" s="76"/>
-      <c r="I6" s="76"/>
+      <c r="G6" s="77"/>
+      <c r="H6" s="77"/>
+      <c r="I6" s="77"/>
     </row>
     <row r="7" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="42"/>
       <c r="C7" s="39"/>
-      <c r="G7" s="76"/>
-      <c r="H7" s="76"/>
-      <c r="I7" s="76"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="77"/>
     </row>
     <row r="8" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="42"/>
       <c r="C8" s="39"/>
-      <c r="G8" s="76"/>
-      <c r="H8" s="76"/>
-      <c r="I8" s="76"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="77"/>
+      <c r="I8" s="77"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B9" s="42"/>
       <c r="C9" s="39"/>
-      <c r="G9" s="76"/>
-      <c r="H9" s="76"/>
-      <c r="I9" s="76"/>
+      <c r="G9" s="77"/>
+      <c r="H9" s="77"/>
+      <c r="I9" s="77"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B10" s="42"/>
       <c r="C10" s="39"/>
-      <c r="G10" s="76"/>
-      <c r="H10" s="76"/>
-      <c r="I10" s="76"/>
+      <c r="G10" s="77"/>
+      <c r="H10" s="77"/>
+      <c r="I10" s="77"/>
     </row>
     <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
@@ -4078,9 +4084,9 @@
       </c>
       <c r="B11" s="42"/>
       <c r="C11" s="39"/>
-      <c r="G11" s="76"/>
-      <c r="H11" s="76"/>
-      <c r="I11" s="76"/>
+      <c r="G11" s="77"/>
+      <c r="H11" s="77"/>
+      <c r="I11" s="77"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B12" s="42"/>
@@ -4104,6 +4110,9 @@
       </c>
       <c r="B16" s="42"/>
       <c r="C16" s="39"/>
+      <c r="G16" s="43" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B17" s="42"/>
@@ -4128,12 +4137,14 @@
       <c r="B21" s="42"/>
       <c r="C21" s="39"/>
     </row>
-    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="B22" s="42"/>
       <c r="C22" s="39"/>
-      <c r="G22" s="77" t="s">
-        <v>35</v>
-      </c>
+      <c r="G22" s="76" t="s">
+        <v>31</v>
+      </c>
+      <c r="H22" s="76"/>
+      <c r="I22" s="76"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B23" s="42"/>
@@ -4142,6 +4153,12 @@
     <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B24" s="42"/>
       <c r="C24" s="39"/>
+      <c r="G24" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="I24" s="31" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B25" s="42"/>
@@ -4158,14 +4175,9 @@
       <c r="B27" s="42"/>
       <c r="C27" s="39"/>
     </row>
-    <row r="28" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B28" s="42"/>
       <c r="C28" s="39"/>
-      <c r="G28" s="75" t="s">
-        <v>31</v>
-      </c>
-      <c r="H28" s="75"/>
-      <c r="I28" s="75"/>
     </row>
     <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B29" s="42"/>
@@ -4288,7 +4300,7 @@
   <mergeCells count="4">
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G22:I22"/>
     <mergeCell ref="G5:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added breast w rework
</commit_message>
<xml_diff>
--- a/CustomLabelPrinter/src/paperwork/recap.xlsx
+++ b/CustomLabelPrinter/src/paperwork/recap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdphu\git\customlabelprinter\CustomLabelPrinter\src\paperwork\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\pdgwinterm7\git\repository\CustomLabelPrinter\src\paperwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7094907F-63B8-41FB-80D0-7BFDC8CA68F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46770C53-1A09-474A-B1D7-0554E57BDDF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8925" yWindow="825" windowWidth="25740" windowHeight="15975" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="10740" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BREAST" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>Green</t>
+  </si>
+  <si>
+    <t>Breast with rework:</t>
   </si>
 </sst>
 </file>
@@ -542,7 +545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -625,6 +628,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -637,6 +643,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -649,11 +661,41 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -679,47 +721,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1024,54 +1030,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="35.25" x14ac:dyDescent="0.25">
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
     </row>
     <row r="2" spans="2:19" ht="27.75" x14ac:dyDescent="0.4">
       <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="45"/>
-      <c r="F2" s="46" t="s">
+      <c r="E2" s="46"/>
+      <c r="F2" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
       <c r="L2" s="7"/>
       <c r="M2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
       <c r="P2" s="7"/>
     </row>
     <row r="3" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
     </row>
     <row r="4" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E4" s="8">
@@ -1104,10 +1110,10 @@
       <c r="N4" s="8">
         <v>26</v>
       </c>
-      <c r="O4" s="47" t="s">
+      <c r="O4" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="47"/>
+      <c r="P4" s="48"/>
       <c r="R4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1908,57 +1914,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="35.25" x14ac:dyDescent="0.25">
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
     </row>
     <row r="2" spans="2:19" ht="27.75" x14ac:dyDescent="0.4">
       <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="45"/>
-      <c r="F2" s="46" t="s">
+      <c r="E2" s="46"/>
+      <c r="F2" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
       <c r="L2" s="7"/>
       <c r="M2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
       <c r="P2" s="7"/>
       <c r="S2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
     </row>
     <row r="4" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E4" s="8">
@@ -1991,10 +1997,10 @@
       <c r="N4" s="8">
         <v>26</v>
       </c>
-      <c r="O4" s="47" t="s">
+      <c r="O4" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="47"/>
+      <c r="P4" s="48"/>
     </row>
     <row r="5" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="15"/>
@@ -2789,54 +2795,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="35.25" x14ac:dyDescent="0.25">
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
     </row>
     <row r="2" spans="2:19" ht="27.75" x14ac:dyDescent="0.4">
       <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="45"/>
-      <c r="F2" s="46" t="s">
+      <c r="E2" s="46"/>
+      <c r="F2" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
       <c r="L2" s="7"/>
       <c r="M2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
       <c r="P2" s="7"/>
     </row>
     <row r="3" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
     </row>
     <row r="4" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E4" s="8">
@@ -2869,20 +2875,20 @@
       <c r="N4" s="8">
         <v>26</v>
       </c>
-      <c r="O4" s="47" t="s">
+      <c r="O4" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="47"/>
+      <c r="P4" s="48"/>
       <c r="S4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="15"/>
-      <c r="C5" s="52">
+      <c r="C5" s="49">
         <v>22486</v>
       </c>
-      <c r="D5" s="53"/>
+      <c r="D5" s="50"/>
       <c r="E5" s="16"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
@@ -2893,13 +2899,13 @@
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
       <c r="N5" s="18"/>
-      <c r="O5" s="54"/>
-      <c r="P5" s="55"/>
+      <c r="O5" s="67"/>
+      <c r="P5" s="68"/>
     </row>
     <row r="6" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="15"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="49"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="52"/>
       <c r="E6" s="19"/>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
@@ -2910,13 +2916,13 @@
       <c r="L6" s="20"/>
       <c r="M6" s="20"/>
       <c r="N6" s="21"/>
-      <c r="O6" s="56"/>
-      <c r="P6" s="57"/>
+      <c r="O6" s="69"/>
+      <c r="P6" s="70"/>
     </row>
     <row r="7" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="15"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="49"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="52"/>
       <c r="E7" s="19"/>
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
@@ -2927,13 +2933,13 @@
       <c r="L7" s="20"/>
       <c r="M7" s="20"/>
       <c r="N7" s="21"/>
-      <c r="O7" s="58"/>
-      <c r="P7" s="59"/>
+      <c r="O7" s="71"/>
+      <c r="P7" s="72"/>
     </row>
     <row r="8" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="15"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="49"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="52"/>
       <c r="E8" s="19"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
@@ -2944,13 +2950,13 @@
       <c r="L8" s="20"/>
       <c r="M8" s="20"/>
       <c r="N8" s="21"/>
-      <c r="O8" s="58"/>
-      <c r="P8" s="59"/>
+      <c r="O8" s="71"/>
+      <c r="P8" s="72"/>
     </row>
     <row r="9" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="15"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="49"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="52"/>
       <c r="E9" s="19"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
@@ -2961,13 +2967,13 @@
       <c r="L9" s="20"/>
       <c r="M9" s="20"/>
       <c r="N9" s="21"/>
-      <c r="O9" s="58"/>
-      <c r="P9" s="59"/>
+      <c r="O9" s="71"/>
+      <c r="P9" s="72"/>
     </row>
     <row r="10" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="15"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="49"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="52"/>
       <c r="E10" s="19"/>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
@@ -2978,13 +2984,13 @@
       <c r="L10" s="20"/>
       <c r="M10" s="20"/>
       <c r="N10" s="21"/>
-      <c r="O10" s="58"/>
-      <c r="P10" s="59"/>
+      <c r="O10" s="71"/>
+      <c r="P10" s="72"/>
     </row>
     <row r="11" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="15"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="49"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="52"/>
       <c r="E11" s="19"/>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
@@ -2995,13 +3001,13 @@
       <c r="L11" s="20"/>
       <c r="M11" s="20"/>
       <c r="N11" s="21"/>
-      <c r="O11" s="58"/>
-      <c r="P11" s="59"/>
+      <c r="O11" s="71"/>
+      <c r="P11" s="72"/>
     </row>
     <row r="12" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="15"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="49"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="52"/>
       <c r="E12" s="19"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
@@ -3012,13 +3018,13 @@
       <c r="L12" s="20"/>
       <c r="M12" s="20"/>
       <c r="N12" s="21"/>
-      <c r="O12" s="58"/>
-      <c r="P12" s="59"/>
+      <c r="O12" s="71"/>
+      <c r="P12" s="72"/>
     </row>
     <row r="13" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="15"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="49"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="52"/>
       <c r="E13" s="19"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
@@ -3029,13 +3035,13 @@
       <c r="L13" s="20"/>
       <c r="M13" s="20"/>
       <c r="N13" s="21"/>
-      <c r="O13" s="58"/>
-      <c r="P13" s="59"/>
+      <c r="O13" s="71"/>
+      <c r="P13" s="72"/>
     </row>
     <row r="14" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="15"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="49"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="52"/>
       <c r="E14" s="19"/>
       <c r="F14" s="20"/>
       <c r="G14" s="20"/>
@@ -3046,13 +3052,13 @@
       <c r="L14" s="20"/>
       <c r="M14" s="20"/>
       <c r="N14" s="21"/>
-      <c r="O14" s="58"/>
-      <c r="P14" s="59"/>
+      <c r="O14" s="71"/>
+      <c r="P14" s="72"/>
     </row>
     <row r="15" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="15"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="49"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="52"/>
       <c r="E15" s="19"/>
       <c r="F15" s="20"/>
       <c r="G15" s="20"/>
@@ -3065,13 +3071,13 @@
       <c r="L15" s="20"/>
       <c r="M15" s="20"/>
       <c r="N15" s="21"/>
-      <c r="O15" s="58"/>
-      <c r="P15" s="59"/>
+      <c r="O15" s="71"/>
+      <c r="P15" s="72"/>
     </row>
     <row r="16" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="15"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="49"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="52"/>
       <c r="E16" s="19"/>
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
@@ -3082,13 +3088,13 @@
       <c r="L16" s="20"/>
       <c r="M16" s="20"/>
       <c r="N16" s="21"/>
-      <c r="O16" s="58"/>
-      <c r="P16" s="59"/>
+      <c r="O16" s="71"/>
+      <c r="P16" s="72"/>
     </row>
     <row r="17" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="15"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="49"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="52"/>
       <c r="E17" s="22"/>
       <c r="F17" s="23"/>
       <c r="G17" s="23"/>
@@ -3099,13 +3105,13 @@
       <c r="L17" s="23"/>
       <c r="M17" s="23"/>
       <c r="N17" s="24"/>
-      <c r="O17" s="58"/>
-      <c r="P17" s="59"/>
+      <c r="O17" s="71"/>
+      <c r="P17" s="72"/>
     </row>
     <row r="18" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="15"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="49"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="52"/>
       <c r="E18" s="11"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
@@ -3116,13 +3122,13 @@
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
       <c r="N18" s="12"/>
-      <c r="O18" s="58"/>
-      <c r="P18" s="59"/>
+      <c r="O18" s="71"/>
+      <c r="P18" s="72"/>
     </row>
     <row r="19" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="15"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="49"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="52"/>
       <c r="E19" s="11"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
@@ -3133,13 +3139,13 @@
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
       <c r="N19" s="12"/>
-      <c r="O19" s="58"/>
-      <c r="P19" s="59"/>
+      <c r="O19" s="71"/>
+      <c r="P19" s="72"/>
     </row>
     <row r="20" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="15"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="52"/>
       <c r="E20" s="11"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
@@ -3150,13 +3156,13 @@
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
       <c r="N20" s="12"/>
-      <c r="O20" s="58"/>
-      <c r="P20" s="59"/>
+      <c r="O20" s="71"/>
+      <c r="P20" s="72"/>
     </row>
     <row r="21" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="15"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="49"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="52"/>
       <c r="E21" s="11"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -3167,13 +3173,13 @@
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
       <c r="N21" s="12"/>
-      <c r="O21" s="58"/>
-      <c r="P21" s="59"/>
+      <c r="O21" s="71"/>
+      <c r="P21" s="72"/>
     </row>
     <row r="22" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="15"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="49"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="52"/>
       <c r="E22" s="11"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -3184,13 +3190,13 @@
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
       <c r="N22" s="12"/>
-      <c r="O22" s="58"/>
-      <c r="P22" s="59"/>
+      <c r="O22" s="71"/>
+      <c r="P22" s="72"/>
     </row>
     <row r="23" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="15"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="49"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="52"/>
       <c r="E23" s="11"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
@@ -3201,13 +3207,13 @@
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
       <c r="N23" s="12"/>
-      <c r="O23" s="58"/>
-      <c r="P23" s="59"/>
+      <c r="O23" s="71"/>
+      <c r="P23" s="72"/>
     </row>
     <row r="24" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="15"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="49"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="52"/>
       <c r="E24" s="11"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -3218,13 +3224,13 @@
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
       <c r="N24" s="12"/>
-      <c r="O24" s="58"/>
-      <c r="P24" s="59"/>
+      <c r="O24" s="71"/>
+      <c r="P24" s="72"/>
     </row>
     <row r="25" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="15"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="49"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="52"/>
       <c r="E25" s="11"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
@@ -3235,13 +3241,13 @@
       <c r="L25" s="9"/>
       <c r="M25" s="9"/>
       <c r="N25" s="12"/>
-      <c r="O25" s="58"/>
-      <c r="P25" s="59"/>
+      <c r="O25" s="71"/>
+      <c r="P25" s="72"/>
     </row>
     <row r="26" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="15"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="49"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="52"/>
       <c r="E26" s="11"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
@@ -3252,13 +3258,13 @@
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
       <c r="N26" s="12"/>
-      <c r="O26" s="58"/>
-      <c r="P26" s="59"/>
+      <c r="O26" s="71"/>
+      <c r="P26" s="72"/>
     </row>
     <row r="27" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="15"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="51"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="54"/>
       <c r="E27" s="4"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -3269,13 +3275,13 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="13"/>
-      <c r="O27" s="60"/>
-      <c r="P27" s="61"/>
+      <c r="O27" s="73"/>
+      <c r="P27" s="74"/>
     </row>
     <row r="28" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="15"/>
-      <c r="C28" s="52"/>
-      <c r="D28" s="53"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="50"/>
       <c r="E28" s="6"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -3286,13 +3292,13 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="10"/>
-      <c r="O28" s="62"/>
-      <c r="P28" s="63"/>
+      <c r="O28" s="55"/>
+      <c r="P28" s="56"/>
     </row>
     <row r="29" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="15"/>
-      <c r="C29" s="48"/>
-      <c r="D29" s="49"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="52"/>
       <c r="E29" s="11"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
@@ -3303,13 +3309,13 @@
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
       <c r="N29" s="12"/>
-      <c r="O29" s="64"/>
-      <c r="P29" s="65"/>
+      <c r="O29" s="57"/>
+      <c r="P29" s="58"/>
     </row>
     <row r="30" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="15"/>
-      <c r="C30" s="48"/>
-      <c r="D30" s="49"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="52"/>
       <c r="E30" s="11"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
@@ -3320,13 +3326,13 @@
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
       <c r="N30" s="12"/>
-      <c r="O30" s="64"/>
-      <c r="P30" s="65"/>
+      <c r="O30" s="57"/>
+      <c r="P30" s="58"/>
     </row>
     <row r="31" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="15"/>
-      <c r="C31" s="48"/>
-      <c r="D31" s="49"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="52"/>
       <c r="E31" s="11"/>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
@@ -3337,13 +3343,13 @@
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
       <c r="N31" s="12"/>
-      <c r="O31" s="64"/>
-      <c r="P31" s="65"/>
+      <c r="O31" s="57"/>
+      <c r="P31" s="58"/>
     </row>
     <row r="32" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="15"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="49"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="52"/>
       <c r="E32" s="11"/>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
@@ -3354,13 +3360,13 @@
       <c r="L32" s="9"/>
       <c r="M32" s="9"/>
       <c r="N32" s="12"/>
-      <c r="O32" s="64"/>
-      <c r="P32" s="65"/>
+      <c r="O32" s="57"/>
+      <c r="P32" s="58"/>
     </row>
     <row r="33" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="15"/>
-      <c r="C33" s="48"/>
-      <c r="D33" s="49"/>
+      <c r="C33" s="51"/>
+      <c r="D33" s="52"/>
       <c r="E33" s="11"/>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
@@ -3371,13 +3377,13 @@
       <c r="L33" s="9"/>
       <c r="M33" s="9"/>
       <c r="N33" s="12"/>
-      <c r="O33" s="64"/>
-      <c r="P33" s="65"/>
+      <c r="O33" s="57"/>
+      <c r="P33" s="58"/>
     </row>
     <row r="34" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="15"/>
-      <c r="C34" s="48"/>
-      <c r="D34" s="49"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="52"/>
       <c r="E34" s="11"/>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
@@ -3388,13 +3394,13 @@
       <c r="L34" s="9"/>
       <c r="M34" s="9"/>
       <c r="N34" s="12"/>
-      <c r="O34" s="64"/>
-      <c r="P34" s="65"/>
+      <c r="O34" s="57"/>
+      <c r="P34" s="58"/>
     </row>
     <row r="35" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="15"/>
-      <c r="C35" s="48"/>
-      <c r="D35" s="49"/>
+      <c r="C35" s="51"/>
+      <c r="D35" s="52"/>
       <c r="E35" s="11"/>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
@@ -3405,13 +3411,13 @@
       <c r="L35" s="9"/>
       <c r="M35" s="9"/>
       <c r="N35" s="12"/>
-      <c r="O35" s="64"/>
-      <c r="P35" s="65"/>
+      <c r="O35" s="57"/>
+      <c r="P35" s="58"/>
     </row>
     <row r="36" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="15"/>
-      <c r="C36" s="48"/>
-      <c r="D36" s="49"/>
+      <c r="C36" s="51"/>
+      <c r="D36" s="52"/>
       <c r="E36" s="11"/>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
@@ -3422,13 +3428,13 @@
       <c r="L36" s="9"/>
       <c r="M36" s="9"/>
       <c r="N36" s="12"/>
-      <c r="O36" s="64"/>
-      <c r="P36" s="65"/>
+      <c r="O36" s="57"/>
+      <c r="P36" s="58"/>
     </row>
     <row r="37" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="15"/>
-      <c r="C37" s="48"/>
-      <c r="D37" s="49"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="52"/>
       <c r="E37" s="11"/>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
@@ -3439,13 +3445,13 @@
       <c r="L37" s="9"/>
       <c r="M37" s="9"/>
       <c r="N37" s="12"/>
-      <c r="O37" s="64"/>
-      <c r="P37" s="65"/>
+      <c r="O37" s="57"/>
+      <c r="P37" s="58"/>
     </row>
     <row r="38" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" s="15"/>
-      <c r="C38" s="50"/>
-      <c r="D38" s="51"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="54"/>
       <c r="E38" s="25"/>
       <c r="F38" s="26"/>
       <c r="G38" s="26"/>
@@ -3456,14 +3462,14 @@
       <c r="L38" s="26"/>
       <c r="M38" s="26"/>
       <c r="N38" s="27"/>
-      <c r="O38" s="66"/>
-      <c r="P38" s="67"/>
+      <c r="O38" s="59"/>
+      <c r="P38" s="60"/>
     </row>
     <row r="39" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39"/>
       <c r="B39"/>
-      <c r="C39" s="68"/>
-      <c r="D39" s="69"/>
+      <c r="C39" s="61"/>
+      <c r="D39" s="62"/>
       <c r="E39" s="29"/>
       <c r="F39" s="28"/>
       <c r="G39" s="28"/>
@@ -3474,8 +3480,8 @@
       <c r="L39" s="28"/>
       <c r="M39" s="28"/>
       <c r="N39" s="30"/>
-      <c r="O39" s="68"/>
-      <c r="P39" s="69"/>
+      <c r="O39" s="61"/>
+      <c r="P39" s="62"/>
       <c r="Q39"/>
       <c r="R39"/>
       <c r="S39"/>
@@ -3483,8 +3489,8 @@
     <row r="40" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40"/>
       <c r="B40"/>
-      <c r="C40" s="70"/>
-      <c r="D40" s="71"/>
+      <c r="C40" s="63"/>
+      <c r="D40" s="64"/>
       <c r="E40" s="29"/>
       <c r="F40" s="28"/>
       <c r="G40" s="28"/>
@@ -3495,8 +3501,8 @@
       <c r="L40" s="28"/>
       <c r="M40" s="28"/>
       <c r="N40" s="30"/>
-      <c r="O40" s="70"/>
-      <c r="P40" s="71"/>
+      <c r="O40" s="63"/>
+      <c r="P40" s="64"/>
       <c r="Q40"/>
       <c r="R40"/>
       <c r="S40"/>
@@ -3504,8 +3510,8 @@
     <row r="41" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41"/>
       <c r="B41"/>
-      <c r="C41" s="70"/>
-      <c r="D41" s="71"/>
+      <c r="C41" s="63"/>
+      <c r="D41" s="64"/>
       <c r="E41" s="29"/>
       <c r="F41" s="28"/>
       <c r="G41" s="28"/>
@@ -3516,8 +3522,8 @@
       <c r="L41" s="28"/>
       <c r="M41" s="28"/>
       <c r="N41" s="30"/>
-      <c r="O41" s="70"/>
-      <c r="P41" s="71"/>
+      <c r="O41" s="63"/>
+      <c r="P41" s="64"/>
       <c r="Q41"/>
       <c r="R41"/>
       <c r="S41"/>
@@ -3525,8 +3531,8 @@
     <row r="42" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42"/>
       <c r="B42"/>
-      <c r="C42" s="70"/>
-      <c r="D42" s="71"/>
+      <c r="C42" s="63"/>
+      <c r="D42" s="64"/>
       <c r="E42" s="29"/>
       <c r="F42" s="28"/>
       <c r="G42" s="28"/>
@@ -3537,8 +3543,8 @@
       <c r="L42" s="28"/>
       <c r="M42" s="28"/>
       <c r="N42" s="30"/>
-      <c r="O42" s="70"/>
-      <c r="P42" s="71"/>
+      <c r="O42" s="63"/>
+      <c r="P42" s="64"/>
       <c r="Q42"/>
       <c r="R42"/>
       <c r="S42"/>
@@ -3546,8 +3552,8 @@
     <row r="43" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43"/>
       <c r="B43"/>
-      <c r="C43" s="72"/>
-      <c r="D43" s="73"/>
+      <c r="C43" s="65"/>
+      <c r="D43" s="66"/>
       <c r="E43" s="29"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
@@ -3558,8 +3564,8 @@
       <c r="L43" s="28"/>
       <c r="M43" s="28"/>
       <c r="N43" s="30"/>
-      <c r="O43" s="72"/>
-      <c r="P43" s="73"/>
+      <c r="O43" s="65"/>
+      <c r="P43" s="66"/>
       <c r="Q43"/>
       <c r="R43"/>
       <c r="S43"/>
@@ -3692,11 +3698,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C28:D29"/>
-    <mergeCell ref="C30:D38"/>
-    <mergeCell ref="O28:P38"/>
-    <mergeCell ref="C39:D43"/>
-    <mergeCell ref="O39:P43"/>
     <mergeCell ref="C1:P1"/>
     <mergeCell ref="F2:K3"/>
     <mergeCell ref="N2:O2"/>
@@ -3706,6 +3707,11 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="O5:P6"/>
     <mergeCell ref="O7:P27"/>
+    <mergeCell ref="C28:D29"/>
+    <mergeCell ref="C30:D38"/>
+    <mergeCell ref="O28:P38"/>
+    <mergeCell ref="C39:D43"/>
+    <mergeCell ref="O39:P43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="35" orientation="portrait" r:id="rId1"/>
@@ -3955,11 +3961,39 @@
       <c r="A31" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="74"/>
-      <c r="C31" s="74"/>
+      <c r="B31" s="76"/>
+      <c r="C31" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="A25:B26"/>
+    <mergeCell ref="C25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:G26"/>
+    <mergeCell ref="H25:I26"/>
+    <mergeCell ref="A27:B28"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:G28"/>
+    <mergeCell ref="H27:I28"/>
+    <mergeCell ref="F19:G20"/>
+    <mergeCell ref="H19:I20"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="C17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:G18"/>
+    <mergeCell ref="H17:I18"/>
+    <mergeCell ref="A21:B22"/>
+    <mergeCell ref="C21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:G22"/>
+    <mergeCell ref="H21:I22"/>
+    <mergeCell ref="A23:B24"/>
+    <mergeCell ref="C23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:G24"/>
+    <mergeCell ref="H23:I24"/>
     <mergeCell ref="F13:G14"/>
     <mergeCell ref="H13:I14"/>
     <mergeCell ref="A15:B16"/>
@@ -3970,34 +4004,6 @@
     <mergeCell ref="A13:B14"/>
     <mergeCell ref="C13:D14"/>
     <mergeCell ref="E13:E14"/>
-    <mergeCell ref="A23:B24"/>
-    <mergeCell ref="C23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:G24"/>
-    <mergeCell ref="H23:I24"/>
-    <mergeCell ref="A21:B22"/>
-    <mergeCell ref="C21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:G22"/>
-    <mergeCell ref="H21:I22"/>
-    <mergeCell ref="F19:G20"/>
-    <mergeCell ref="H19:I20"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="C17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:G18"/>
-    <mergeCell ref="H17:I18"/>
-    <mergeCell ref="H25:I26"/>
-    <mergeCell ref="A27:B28"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:G28"/>
-    <mergeCell ref="H27:I28"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="A25:B26"/>
-    <mergeCell ref="C25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:G26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4008,8 +4014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A016E41C-E536-466F-8BCC-D27E2EA7F174}">
   <dimension ref="A3:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4023,22 +4029,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="G3" s="76" t="s">
+      <c r="B3" s="77"/>
+      <c r="G3" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
     </row>
     <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G5" s="77" t="s">
+      <c r="G5" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="78"/>
     </row>
     <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="40" t="s">
@@ -4046,37 +4052,40 @@
       </c>
       <c r="B6" s="42"/>
       <c r="C6" s="39"/>
-      <c r="G6" s="77"/>
-      <c r="H6" s="77"/>
-      <c r="I6" s="77"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="78"/>
+      <c r="I6" s="78"/>
     </row>
     <row r="7" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="42"/>
       <c r="C7" s="39"/>
-      <c r="G7" s="77"/>
-      <c r="H7" s="77"/>
-      <c r="I7" s="77"/>
-    </row>
-    <row r="8" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G7" s="78"/>
+      <c r="H7" s="78"/>
+      <c r="I7" s="78"/>
+    </row>
+    <row r="8" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="40" t="s">
+        <v>38</v>
+      </c>
       <c r="B8" s="42"/>
-      <c r="C8" s="39"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="77"/>
-      <c r="I8" s="77"/>
+      <c r="C8" s="44"/>
+      <c r="G8" s="78"/>
+      <c r="H8" s="78"/>
+      <c r="I8" s="78"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B9" s="42"/>
       <c r="C9" s="39"/>
-      <c r="G9" s="77"/>
-      <c r="H9" s="77"/>
-      <c r="I9" s="77"/>
+      <c r="G9" s="78"/>
+      <c r="H9" s="78"/>
+      <c r="I9" s="78"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B10" s="42"/>
       <c r="C10" s="39"/>
-      <c r="G10" s="77"/>
-      <c r="H10" s="77"/>
-      <c r="I10" s="77"/>
+      <c r="G10" s="78"/>
+      <c r="H10" s="78"/>
+      <c r="I10" s="78"/>
     </row>
     <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
@@ -4084,9 +4093,9 @@
       </c>
       <c r="B11" s="42"/>
       <c r="C11" s="39"/>
-      <c r="G11" s="77"/>
-      <c r="H11" s="77"/>
-      <c r="I11" s="77"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="78"/>
+      <c r="I11" s="78"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B12" s="42"/>
@@ -4140,11 +4149,11 @@
     <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="B22" s="42"/>
       <c r="C22" s="39"/>
-      <c r="G22" s="76" t="s">
+      <c r="G22" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="H22" s="76"/>
-      <c r="I22" s="76"/>
+      <c r="H22" s="77"/>
+      <c r="I22" s="77"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B23" s="42"/>

</xml_diff>

<commit_message>
adjusted rework issued position
</commit_message>
<xml_diff>
--- a/CustomLabelPrinter/src/paperwork/recap.xlsx
+++ b/CustomLabelPrinter/src/paperwork/recap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\pdgwinterm7\git\repository\CustomLabelPrinter\src\paperwork\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdphu\git\customlabelprinter\CustomLabelPrinter\src\paperwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F494FD4-E7F9-45B9-91A0-032F7A2DF408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD845C9D-5435-4812-A75B-15467F296864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="10740" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2850" yWindow="960" windowWidth="25740" windowHeight="15975" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BREAST" sheetId="1" r:id="rId1"/>
@@ -542,7 +542,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -628,6 +628,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -640,6 +643,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -652,11 +661,41 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -682,47 +721,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1027,54 +1030,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="35.25" x14ac:dyDescent="0.25">
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
     </row>
     <row r="2" spans="2:19" ht="27.75" x14ac:dyDescent="0.4">
       <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="46"/>
-      <c r="F2" s="47" t="s">
+      <c r="E2" s="47"/>
+      <c r="F2" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
       <c r="L2" s="7"/>
       <c r="M2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
       <c r="P2" s="7"/>
     </row>
     <row r="3" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
     </row>
     <row r="4" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E4" s="8">
@@ -1107,10 +1110,10 @@
       <c r="N4" s="8">
         <v>26</v>
       </c>
-      <c r="O4" s="48" t="s">
+      <c r="O4" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="48"/>
+      <c r="P4" s="49"/>
       <c r="R4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1911,57 +1914,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="35.25" x14ac:dyDescent="0.25">
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
     </row>
     <row r="2" spans="2:19" ht="27.75" x14ac:dyDescent="0.4">
       <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="46"/>
-      <c r="F2" s="47" t="s">
+      <c r="E2" s="47"/>
+      <c r="F2" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
       <c r="L2" s="7"/>
       <c r="M2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
       <c r="P2" s="7"/>
       <c r="S2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
     </row>
     <row r="4" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E4" s="8">
@@ -1994,10 +1997,10 @@
       <c r="N4" s="8">
         <v>26</v>
       </c>
-      <c r="O4" s="48" t="s">
+      <c r="O4" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="48"/>
+      <c r="P4" s="49"/>
     </row>
     <row r="5" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="15"/>
@@ -2792,54 +2795,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="35.25" x14ac:dyDescent="0.25">
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
     </row>
     <row r="2" spans="2:19" ht="27.75" x14ac:dyDescent="0.4">
       <c r="C2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="46"/>
-      <c r="F2" s="47" t="s">
+      <c r="E2" s="47"/>
+      <c r="F2" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
       <c r="L2" s="7"/>
       <c r="M2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
       <c r="P2" s="7"/>
     </row>
     <row r="3" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
     </row>
     <row r="4" spans="2:19" s="1" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E4" s="8">
@@ -2872,20 +2875,20 @@
       <c r="N4" s="8">
         <v>26</v>
       </c>
-      <c r="O4" s="48" t="s">
+      <c r="O4" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="48"/>
+      <c r="P4" s="49"/>
       <c r="S4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="15"/>
-      <c r="C5" s="53">
+      <c r="C5" s="50">
         <v>22486</v>
       </c>
-      <c r="D5" s="54"/>
+      <c r="D5" s="51"/>
       <c r="E5" s="16"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
@@ -2896,13 +2899,13 @@
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
       <c r="N5" s="18"/>
-      <c r="O5" s="55"/>
-      <c r="P5" s="56"/>
+      <c r="O5" s="68"/>
+      <c r="P5" s="69"/>
     </row>
     <row r="6" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="15"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="50"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="53"/>
       <c r="E6" s="19"/>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
@@ -2913,13 +2916,13 @@
       <c r="L6" s="20"/>
       <c r="M6" s="20"/>
       <c r="N6" s="21"/>
-      <c r="O6" s="57"/>
-      <c r="P6" s="58"/>
+      <c r="O6" s="70"/>
+      <c r="P6" s="71"/>
     </row>
     <row r="7" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="15"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="50"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="53"/>
       <c r="E7" s="19"/>
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
@@ -2930,13 +2933,13 @@
       <c r="L7" s="20"/>
       <c r="M7" s="20"/>
       <c r="N7" s="21"/>
-      <c r="O7" s="59"/>
-      <c r="P7" s="60"/>
+      <c r="O7" s="72"/>
+      <c r="P7" s="73"/>
     </row>
     <row r="8" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="15"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="50"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="53"/>
       <c r="E8" s="19"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
@@ -2947,13 +2950,13 @@
       <c r="L8" s="20"/>
       <c r="M8" s="20"/>
       <c r="N8" s="21"/>
-      <c r="O8" s="59"/>
-      <c r="P8" s="60"/>
+      <c r="O8" s="72"/>
+      <c r="P8" s="73"/>
     </row>
     <row r="9" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="15"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="50"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="53"/>
       <c r="E9" s="19"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
@@ -2964,13 +2967,13 @@
       <c r="L9" s="20"/>
       <c r="M9" s="20"/>
       <c r="N9" s="21"/>
-      <c r="O9" s="59"/>
-      <c r="P9" s="60"/>
+      <c r="O9" s="72"/>
+      <c r="P9" s="73"/>
     </row>
     <row r="10" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="15"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="50"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="53"/>
       <c r="E10" s="19"/>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
@@ -2981,13 +2984,13 @@
       <c r="L10" s="20"/>
       <c r="M10" s="20"/>
       <c r="N10" s="21"/>
-      <c r="O10" s="59"/>
-      <c r="P10" s="60"/>
+      <c r="O10" s="72"/>
+      <c r="P10" s="73"/>
     </row>
     <row r="11" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="15"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="50"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="53"/>
       <c r="E11" s="19"/>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
@@ -2998,13 +3001,13 @@
       <c r="L11" s="20"/>
       <c r="M11" s="20"/>
       <c r="N11" s="21"/>
-      <c r="O11" s="59"/>
-      <c r="P11" s="60"/>
+      <c r="O11" s="72"/>
+      <c r="P11" s="73"/>
     </row>
     <row r="12" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="15"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="50"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="53"/>
       <c r="E12" s="19"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
@@ -3015,13 +3018,13 @@
       <c r="L12" s="20"/>
       <c r="M12" s="20"/>
       <c r="N12" s="21"/>
-      <c r="O12" s="59"/>
-      <c r="P12" s="60"/>
+      <c r="O12" s="72"/>
+      <c r="P12" s="73"/>
     </row>
     <row r="13" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="15"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="50"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="53"/>
       <c r="E13" s="19"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
@@ -3032,13 +3035,13 @@
       <c r="L13" s="20"/>
       <c r="M13" s="20"/>
       <c r="N13" s="21"/>
-      <c r="O13" s="59"/>
-      <c r="P13" s="60"/>
+      <c r="O13" s="72"/>
+      <c r="P13" s="73"/>
     </row>
     <row r="14" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="15"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="50"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="53"/>
       <c r="E14" s="19"/>
       <c r="F14" s="20"/>
       <c r="G14" s="20"/>
@@ -3049,13 +3052,13 @@
       <c r="L14" s="20"/>
       <c r="M14" s="20"/>
       <c r="N14" s="21"/>
-      <c r="O14" s="59"/>
-      <c r="P14" s="60"/>
+      <c r="O14" s="72"/>
+      <c r="P14" s="73"/>
     </row>
     <row r="15" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="15"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="50"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="53"/>
       <c r="E15" s="19"/>
       <c r="F15" s="20"/>
       <c r="G15" s="20"/>
@@ -3068,13 +3071,13 @@
       <c r="L15" s="20"/>
       <c r="M15" s="20"/>
       <c r="N15" s="21"/>
-      <c r="O15" s="59"/>
-      <c r="P15" s="60"/>
+      <c r="O15" s="72"/>
+      <c r="P15" s="73"/>
     </row>
     <row r="16" spans="2:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="15"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="50"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="53"/>
       <c r="E16" s="19"/>
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
@@ -3085,13 +3088,13 @@
       <c r="L16" s="20"/>
       <c r="M16" s="20"/>
       <c r="N16" s="21"/>
-      <c r="O16" s="59"/>
-      <c r="P16" s="60"/>
+      <c r="O16" s="72"/>
+      <c r="P16" s="73"/>
     </row>
     <row r="17" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="15"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="50"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="53"/>
       <c r="E17" s="22"/>
       <c r="F17" s="23"/>
       <c r="G17" s="23"/>
@@ -3102,13 +3105,13 @@
       <c r="L17" s="23"/>
       <c r="M17" s="23"/>
       <c r="N17" s="24"/>
-      <c r="O17" s="59"/>
-      <c r="P17" s="60"/>
+      <c r="O17" s="72"/>
+      <c r="P17" s="73"/>
     </row>
     <row r="18" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="15"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="50"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="53"/>
       <c r="E18" s="11"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
@@ -3119,13 +3122,13 @@
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
       <c r="N18" s="12"/>
-      <c r="O18" s="59"/>
-      <c r="P18" s="60"/>
+      <c r="O18" s="72"/>
+      <c r="P18" s="73"/>
     </row>
     <row r="19" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="15"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="50"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="53"/>
       <c r="E19" s="11"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
@@ -3136,13 +3139,13 @@
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
       <c r="N19" s="12"/>
-      <c r="O19" s="59"/>
-      <c r="P19" s="60"/>
+      <c r="O19" s="72"/>
+      <c r="P19" s="73"/>
     </row>
     <row r="20" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="15"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="50"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="53"/>
       <c r="E20" s="11"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
@@ -3153,13 +3156,13 @@
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
       <c r="N20" s="12"/>
-      <c r="O20" s="59"/>
-      <c r="P20" s="60"/>
+      <c r="O20" s="72"/>
+      <c r="P20" s="73"/>
     </row>
     <row r="21" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="15"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="50"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="53"/>
       <c r="E21" s="11"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -3170,13 +3173,13 @@
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
       <c r="N21" s="12"/>
-      <c r="O21" s="59"/>
-      <c r="P21" s="60"/>
+      <c r="O21" s="72"/>
+      <c r="P21" s="73"/>
     </row>
     <row r="22" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="15"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="50"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="53"/>
       <c r="E22" s="11"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -3187,13 +3190,13 @@
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
       <c r="N22" s="12"/>
-      <c r="O22" s="59"/>
-      <c r="P22" s="60"/>
+      <c r="O22" s="72"/>
+      <c r="P22" s="73"/>
     </row>
     <row r="23" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="15"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="50"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="53"/>
       <c r="E23" s="11"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
@@ -3204,13 +3207,13 @@
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
       <c r="N23" s="12"/>
-      <c r="O23" s="59"/>
-      <c r="P23" s="60"/>
+      <c r="O23" s="72"/>
+      <c r="P23" s="73"/>
     </row>
     <row r="24" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="15"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="50"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="53"/>
       <c r="E24" s="11"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -3221,13 +3224,13 @@
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
       <c r="N24" s="12"/>
-      <c r="O24" s="59"/>
-      <c r="P24" s="60"/>
+      <c r="O24" s="72"/>
+      <c r="P24" s="73"/>
     </row>
     <row r="25" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="15"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="50"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="53"/>
       <c r="E25" s="11"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
@@ -3238,13 +3241,13 @@
       <c r="L25" s="9"/>
       <c r="M25" s="9"/>
       <c r="N25" s="12"/>
-      <c r="O25" s="59"/>
-      <c r="P25" s="60"/>
+      <c r="O25" s="72"/>
+      <c r="P25" s="73"/>
     </row>
     <row r="26" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="15"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="50"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="53"/>
       <c r="E26" s="11"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
@@ -3255,13 +3258,13 @@
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
       <c r="N26" s="12"/>
-      <c r="O26" s="59"/>
-      <c r="P26" s="60"/>
+      <c r="O26" s="72"/>
+      <c r="P26" s="73"/>
     </row>
     <row r="27" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="15"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="52"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="55"/>
       <c r="E27" s="4"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -3272,13 +3275,13 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="13"/>
-      <c r="O27" s="61"/>
-      <c r="P27" s="62"/>
+      <c r="O27" s="74"/>
+      <c r="P27" s="75"/>
     </row>
     <row r="28" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="15"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="54"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="51"/>
       <c r="E28" s="6"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -3289,13 +3292,13 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="10"/>
-      <c r="O28" s="63"/>
-      <c r="P28" s="64"/>
+      <c r="O28" s="56"/>
+      <c r="P28" s="57"/>
     </row>
     <row r="29" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="15"/>
-      <c r="C29" s="49"/>
-      <c r="D29" s="50"/>
+      <c r="C29" s="52"/>
+      <c r="D29" s="53"/>
       <c r="E29" s="11"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
@@ -3306,13 +3309,13 @@
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
       <c r="N29" s="12"/>
-      <c r="O29" s="65"/>
-      <c r="P29" s="66"/>
+      <c r="O29" s="58"/>
+      <c r="P29" s="59"/>
     </row>
     <row r="30" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="15"/>
-      <c r="C30" s="49"/>
-      <c r="D30" s="50"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="53"/>
       <c r="E30" s="11"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
@@ -3323,13 +3326,13 @@
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
       <c r="N30" s="12"/>
-      <c r="O30" s="65"/>
-      <c r="P30" s="66"/>
+      <c r="O30" s="58"/>
+      <c r="P30" s="59"/>
     </row>
     <row r="31" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="15"/>
-      <c r="C31" s="49"/>
-      <c r="D31" s="50"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="53"/>
       <c r="E31" s="11"/>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
@@ -3340,13 +3343,13 @@
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
       <c r="N31" s="12"/>
-      <c r="O31" s="65"/>
-      <c r="P31" s="66"/>
+      <c r="O31" s="58"/>
+      <c r="P31" s="59"/>
     </row>
     <row r="32" spans="2:16" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="15"/>
-      <c r="C32" s="49"/>
-      <c r="D32" s="50"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="53"/>
       <c r="E32" s="11"/>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
@@ -3357,13 +3360,13 @@
       <c r="L32" s="9"/>
       <c r="M32" s="9"/>
       <c r="N32" s="12"/>
-      <c r="O32" s="65"/>
-      <c r="P32" s="66"/>
+      <c r="O32" s="58"/>
+      <c r="P32" s="59"/>
     </row>
     <row r="33" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="15"/>
-      <c r="C33" s="49"/>
-      <c r="D33" s="50"/>
+      <c r="C33" s="52"/>
+      <c r="D33" s="53"/>
       <c r="E33" s="11"/>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
@@ -3374,13 +3377,13 @@
       <c r="L33" s="9"/>
       <c r="M33" s="9"/>
       <c r="N33" s="12"/>
-      <c r="O33" s="65"/>
-      <c r="P33" s="66"/>
+      <c r="O33" s="58"/>
+      <c r="P33" s="59"/>
     </row>
     <row r="34" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="15"/>
-      <c r="C34" s="49"/>
-      <c r="D34" s="50"/>
+      <c r="C34" s="52"/>
+      <c r="D34" s="53"/>
       <c r="E34" s="11"/>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
@@ -3391,13 +3394,13 @@
       <c r="L34" s="9"/>
       <c r="M34" s="9"/>
       <c r="N34" s="12"/>
-      <c r="O34" s="65"/>
-      <c r="P34" s="66"/>
+      <c r="O34" s="58"/>
+      <c r="P34" s="59"/>
     </row>
     <row r="35" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="15"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="50"/>
+      <c r="C35" s="52"/>
+      <c r="D35" s="53"/>
       <c r="E35" s="11"/>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
@@ -3408,13 +3411,13 @@
       <c r="L35" s="9"/>
       <c r="M35" s="9"/>
       <c r="N35" s="12"/>
-      <c r="O35" s="65"/>
-      <c r="P35" s="66"/>
+      <c r="O35" s="58"/>
+      <c r="P35" s="59"/>
     </row>
     <row r="36" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="15"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="50"/>
+      <c r="C36" s="52"/>
+      <c r="D36" s="53"/>
       <c r="E36" s="11"/>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
@@ -3425,13 +3428,13 @@
       <c r="L36" s="9"/>
       <c r="M36" s="9"/>
       <c r="N36" s="12"/>
-      <c r="O36" s="65"/>
-      <c r="P36" s="66"/>
+      <c r="O36" s="58"/>
+      <c r="P36" s="59"/>
     </row>
     <row r="37" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="15"/>
-      <c r="C37" s="49"/>
-      <c r="D37" s="50"/>
+      <c r="C37" s="52"/>
+      <c r="D37" s="53"/>
       <c r="E37" s="11"/>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
@@ -3442,13 +3445,13 @@
       <c r="L37" s="9"/>
       <c r="M37" s="9"/>
       <c r="N37" s="12"/>
-      <c r="O37" s="65"/>
-      <c r="P37" s="66"/>
+      <c r="O37" s="58"/>
+      <c r="P37" s="59"/>
     </row>
     <row r="38" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" s="15"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="52"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="55"/>
       <c r="E38" s="25"/>
       <c r="F38" s="26"/>
       <c r="G38" s="26"/>
@@ -3459,14 +3462,14 @@
       <c r="L38" s="26"/>
       <c r="M38" s="26"/>
       <c r="N38" s="27"/>
-      <c r="O38" s="67"/>
-      <c r="P38" s="68"/>
+      <c r="O38" s="60"/>
+      <c r="P38" s="61"/>
     </row>
     <row r="39" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39"/>
       <c r="B39"/>
-      <c r="C39" s="69"/>
-      <c r="D39" s="70"/>
+      <c r="C39" s="62"/>
+      <c r="D39" s="63"/>
       <c r="E39" s="29"/>
       <c r="F39" s="28"/>
       <c r="G39" s="28"/>
@@ -3477,8 +3480,8 @@
       <c r="L39" s="28"/>
       <c r="M39" s="28"/>
       <c r="N39" s="30"/>
-      <c r="O39" s="69"/>
-      <c r="P39" s="70"/>
+      <c r="O39" s="62"/>
+      <c r="P39" s="63"/>
       <c r="Q39"/>
       <c r="R39"/>
       <c r="S39"/>
@@ -3486,8 +3489,8 @@
     <row r="40" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40"/>
       <c r="B40"/>
-      <c r="C40" s="71"/>
-      <c r="D40" s="72"/>
+      <c r="C40" s="64"/>
+      <c r="D40" s="65"/>
       <c r="E40" s="29"/>
       <c r="F40" s="28"/>
       <c r="G40" s="28"/>
@@ -3498,8 +3501,8 @@
       <c r="L40" s="28"/>
       <c r="M40" s="28"/>
       <c r="N40" s="30"/>
-      <c r="O40" s="71"/>
-      <c r="P40" s="72"/>
+      <c r="O40" s="64"/>
+      <c r="P40" s="65"/>
       <c r="Q40"/>
       <c r="R40"/>
       <c r="S40"/>
@@ -3507,8 +3510,8 @@
     <row r="41" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41"/>
       <c r="B41"/>
-      <c r="C41" s="71"/>
-      <c r="D41" s="72"/>
+      <c r="C41" s="64"/>
+      <c r="D41" s="65"/>
       <c r="E41" s="29"/>
       <c r="F41" s="28"/>
       <c r="G41" s="28"/>
@@ -3519,8 +3522,8 @@
       <c r="L41" s="28"/>
       <c r="M41" s="28"/>
       <c r="N41" s="30"/>
-      <c r="O41" s="71"/>
-      <c r="P41" s="72"/>
+      <c r="O41" s="64"/>
+      <c r="P41" s="65"/>
       <c r="Q41"/>
       <c r="R41"/>
       <c r="S41"/>
@@ -3528,8 +3531,8 @@
     <row r="42" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42"/>
       <c r="B42"/>
-      <c r="C42" s="71"/>
-      <c r="D42" s="72"/>
+      <c r="C42" s="64"/>
+      <c r="D42" s="65"/>
       <c r="E42" s="29"/>
       <c r="F42" s="28"/>
       <c r="G42" s="28"/>
@@ -3540,8 +3543,8 @@
       <c r="L42" s="28"/>
       <c r="M42" s="28"/>
       <c r="N42" s="30"/>
-      <c r="O42" s="71"/>
-      <c r="P42" s="72"/>
+      <c r="O42" s="64"/>
+      <c r="P42" s="65"/>
       <c r="Q42"/>
       <c r="R42"/>
       <c r="S42"/>
@@ -3549,8 +3552,8 @@
     <row r="43" spans="1:19" s="1" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43"/>
       <c r="B43"/>
-      <c r="C43" s="73"/>
-      <c r="D43" s="74"/>
+      <c r="C43" s="66"/>
+      <c r="D43" s="67"/>
       <c r="E43" s="29"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
@@ -3561,8 +3564,8 @@
       <c r="L43" s="28"/>
       <c r="M43" s="28"/>
       <c r="N43" s="30"/>
-      <c r="O43" s="73"/>
-      <c r="P43" s="74"/>
+      <c r="O43" s="66"/>
+      <c r="P43" s="67"/>
       <c r="Q43"/>
       <c r="R43"/>
       <c r="S43"/>
@@ -3695,11 +3698,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C28:D29"/>
-    <mergeCell ref="C30:D38"/>
-    <mergeCell ref="O28:P38"/>
-    <mergeCell ref="C39:D43"/>
-    <mergeCell ref="O39:P43"/>
     <mergeCell ref="C1:P1"/>
     <mergeCell ref="F2:K3"/>
     <mergeCell ref="N2:O2"/>
@@ -3709,6 +3707,11 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="O5:P6"/>
     <mergeCell ref="O7:P27"/>
+    <mergeCell ref="C28:D29"/>
+    <mergeCell ref="C30:D38"/>
+    <mergeCell ref="O28:P38"/>
+    <mergeCell ref="C39:D43"/>
+    <mergeCell ref="O39:P43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="35" orientation="portrait" r:id="rId1"/>
@@ -3958,11 +3961,39 @@
       <c r="A31" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="75"/>
-      <c r="C31" s="75"/>
+      <c r="B31" s="77"/>
+      <c r="C31" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="A25:B26"/>
+    <mergeCell ref="C25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:G26"/>
+    <mergeCell ref="H25:I26"/>
+    <mergeCell ref="A27:B28"/>
+    <mergeCell ref="C27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:G28"/>
+    <mergeCell ref="H27:I28"/>
+    <mergeCell ref="F19:G20"/>
+    <mergeCell ref="H19:I20"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="C17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:G18"/>
+    <mergeCell ref="H17:I18"/>
+    <mergeCell ref="A21:B22"/>
+    <mergeCell ref="C21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:G22"/>
+    <mergeCell ref="H21:I22"/>
+    <mergeCell ref="A23:B24"/>
+    <mergeCell ref="C23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:G24"/>
+    <mergeCell ref="H23:I24"/>
     <mergeCell ref="F13:G14"/>
     <mergeCell ref="H13:I14"/>
     <mergeCell ref="A15:B16"/>
@@ -3973,34 +4004,6 @@
     <mergeCell ref="A13:B14"/>
     <mergeCell ref="C13:D14"/>
     <mergeCell ref="E13:E14"/>
-    <mergeCell ref="A23:B24"/>
-    <mergeCell ref="C23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:G24"/>
-    <mergeCell ref="H23:I24"/>
-    <mergeCell ref="A21:B22"/>
-    <mergeCell ref="C21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:G22"/>
-    <mergeCell ref="H21:I22"/>
-    <mergeCell ref="F19:G20"/>
-    <mergeCell ref="H19:I20"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="C17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:G18"/>
-    <mergeCell ref="H17:I18"/>
-    <mergeCell ref="H25:I26"/>
-    <mergeCell ref="A27:B28"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:G28"/>
-    <mergeCell ref="H27:I28"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="A25:B26"/>
-    <mergeCell ref="C25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:G26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4012,7 +4015,7 @@
   <dimension ref="A3:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G7" sqref="G7:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4026,22 +4029,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="77"/>
-      <c r="G3" s="77" t="s">
+      <c r="B3" s="78"/>
+      <c r="G3" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
     </row>
     <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G5" s="78" t="s">
+      <c r="G5" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
     </row>
     <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="40" t="s">
@@ -4049,38 +4052,38 @@
       </c>
       <c r="B6" s="42"/>
       <c r="C6" s="39"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="78"/>
+      <c r="G6" s="79"/>
+      <c r="H6" s="79"/>
+      <c r="I6" s="79"/>
     </row>
     <row r="7" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="42"/>
       <c r="C7" s="39"/>
-      <c r="G7" s="78"/>
-      <c r="H7" s="78"/>
-      <c r="I7" s="78"/>
+      <c r="G7" s="79"/>
+      <c r="H7" s="79"/>
+      <c r="I7" s="79"/>
     </row>
     <row r="8" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="40"/>
       <c r="B8" s="42"/>
       <c r="C8" s="44"/>
-      <c r="G8" s="78"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="78"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B9" s="42"/>
       <c r="C9" s="39"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="78"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B10" s="42"/>
       <c r="C10" s="39"/>
-      <c r="G10" s="78"/>
-      <c r="H10" s="78"/>
-      <c r="I10" s="78"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
     </row>
     <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
@@ -4088,9 +4091,9 @@
       </c>
       <c r="B11" s="42"/>
       <c r="C11" s="39"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="78"/>
-      <c r="I11" s="78"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B12" s="42"/>
@@ -4144,11 +4147,11 @@
     <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="B22" s="42"/>
       <c r="C22" s="39"/>
-      <c r="G22" s="77" t="s">
+      <c r="G22" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="H22" s="77"/>
-      <c r="I22" s="77"/>
+      <c r="H22" s="78"/>
+      <c r="I22" s="78"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B23" s="42"/>
@@ -4301,11 +4304,12 @@
       <c r="C45" s="39"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="G3:I3"/>
     <mergeCell ref="G22:I22"/>
-    <mergeCell ref="G5:I11"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>